<commit_message>
analyzer done without cross validation
</commit_message>
<xml_diff>
--- a/Liushui/output/sample1.xlsx
+++ b/Liushui/output/sample1.xlsx
@@ -477,9 +477,7 @@
       <c r="M2" t="n">
         <v>327470.96</v>
       </c>
-      <c r="N2" t="n">
-        <v>20190202</v>
-      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -521,9 +519,7 @@
       <c r="M3" t="n">
         <v>327464.45</v>
       </c>
-      <c r="N3" t="n">
-        <v>20190202</v>
-      </c>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -565,9 +561,7 @@
       <c r="M4" t="n">
         <v>327414.45</v>
       </c>
-      <c r="N4" t="n">
-        <v>20190202</v>
-      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -609,9 +603,7 @@
       <c r="M5" t="n">
         <v>280822.45</v>
       </c>
-      <c r="N5" t="n">
-        <v>20190212</v>
-      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -653,9 +645,7 @@
       <c r="M6" t="n">
         <v>265142.45</v>
       </c>
-      <c r="N6" t="n">
-        <v>20190213</v>
-      </c>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -705,9 +695,7 @@
       <c r="M7" t="n">
         <v>240656.65</v>
       </c>
-      <c r="N7" t="n">
-        <v>20190213</v>
-      </c>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -753,9 +741,7 @@
       <c r="M8" t="n">
         <v>237238.92</v>
       </c>
-      <c r="N8" t="n">
-        <v>20190215</v>
-      </c>
+      <c r="N8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -797,9 +783,7 @@
       <c r="M9" t="n">
         <v>237229.61</v>
       </c>
-      <c r="N9" t="n">
-        <v>20190302</v>
-      </c>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -841,9 +825,7 @@
       <c r="M10" t="n">
         <v>237179.61</v>
       </c>
-      <c r="N10" t="n">
-        <v>20190302</v>
-      </c>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -893,9 +875,7 @@
       <c r="M11" t="n">
         <v>224936.71</v>
       </c>
-      <c r="N11" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -945,9 +925,7 @@
       <c r="M12" t="n">
         <v>211492.58</v>
       </c>
-      <c r="N12" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -997,9 +975,7 @@
       <c r="M13" t="n">
         <v>198138.45</v>
       </c>
-      <c r="N13" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1049,9 +1025,7 @@
       <c r="M14" t="n">
         <v>181344.32</v>
       </c>
-      <c r="N14" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1101,9 +1075,7 @@
       <c r="M15" t="n">
         <v>170746.07</v>
       </c>
-      <c r="N15" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1153,9 +1125,7 @@
       <c r="M16" t="n">
         <v>147601.94</v>
       </c>
-      <c r="N16" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1205,9 +1175,7 @@
       <c r="M17" t="n">
         <v>116983.56</v>
       </c>
-      <c r="N17" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1257,9 +1225,7 @@
       <c r="M18" t="n">
         <v>83709.17999999999</v>
       </c>
-      <c r="N18" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1309,9 +1275,7 @@
       <c r="M19" t="n">
         <v>56565.76</v>
       </c>
-      <c r="N19" t="n">
-        <v>20190311</v>
-      </c>
+      <c r="N19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1353,9 +1317,7 @@
       <c r="M20" t="n">
         <v>9973.76</v>
       </c>
-      <c r="N20" t="n">
-        <v>20190312</v>
-      </c>
+      <c r="N20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1401,9 +1363,7 @@
       <c r="M21" t="n">
         <v>4421.31</v>
       </c>
-      <c r="N21" t="n">
-        <v>20190312</v>
-      </c>
+      <c r="N21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1453,9 +1413,7 @@
       <c r="M22" t="n">
         <v>304421.31</v>
       </c>
-      <c r="N22" t="n">
-        <v>20190314</v>
-      </c>
+      <c r="N22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1505,9 +1463,7 @@
       <c r="M23" t="n">
         <v>164421.31</v>
       </c>
-      <c r="N23" t="n">
-        <v>20190314</v>
-      </c>
+      <c r="N23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1549,9 +1505,7 @@
       <c r="M24" t="n">
         <v>148741.31</v>
       </c>
-      <c r="N24" t="n">
-        <v>20190314</v>
-      </c>
+      <c r="N24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1601,9 +1555,7 @@
       <c r="M25" t="n">
         <v>648741.3100000001</v>
       </c>
-      <c r="N25" t="n">
-        <v>20190318</v>
-      </c>
+      <c r="N25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1653,9 +1605,7 @@
       <c r="M26" t="n">
         <v>648740.3100000001</v>
       </c>
-      <c r="N26" t="n">
-        <v>20190319</v>
-      </c>
+      <c r="N26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1701,9 +1651,7 @@
       <c r="M27" t="n">
         <v>648741.3100000001</v>
       </c>
-      <c r="N27" t="n">
-        <v>20190320</v>
-      </c>
+      <c r="N27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1745,9 +1693,7 @@
       <c r="M28" t="n">
         <v>648862.21</v>
       </c>
-      <c r="N28" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1797,9 +1743,7 @@
       <c r="M29" t="n">
         <v>613472.01</v>
       </c>
-      <c r="N29" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1849,9 +1793,7 @@
       <c r="M30" t="n">
         <v>601904.21</v>
       </c>
-      <c r="N30" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1901,9 +1843,7 @@
       <c r="M31" t="n">
         <v>586219.6</v>
       </c>
-      <c r="N31" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1953,9 +1893,7 @@
       <c r="M32" t="n">
         <v>573671.3</v>
       </c>
-      <c r="N32" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2005,9 +1943,7 @@
       <c r="M33" t="n">
         <v>572926.5</v>
       </c>
-      <c r="N33" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2057,9 +1993,7 @@
       <c r="M34" t="n">
         <v>564734.5</v>
       </c>
-      <c r="N34" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2109,9 +2043,7 @@
       <c r="M35" t="n">
         <v>564190.9</v>
       </c>
-      <c r="N35" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2161,9 +2093,7 @@
       <c r="M36" t="n">
         <v>563297.1</v>
       </c>
-      <c r="N36" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2213,9 +2143,7 @@
       <c r="M37" t="n">
         <v>63297.1</v>
       </c>
-      <c r="N37" t="n">
-        <v>20190321</v>
-      </c>
+      <c r="N37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2257,9 +2185,7 @@
       <c r="M38" t="n">
         <v>63217.95</v>
       </c>
-      <c r="N38" t="n">
-        <v>20190402</v>
-      </c>
+      <c r="N38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2301,9 +2227,7 @@
       <c r="M39" t="n">
         <v>63206.79</v>
       </c>
-      <c r="N39" t="n">
-        <v>20190402</v>
-      </c>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2345,9 +2269,7 @@
       <c r="M40" t="n">
         <v>63156.79</v>
       </c>
-      <c r="N40" t="n">
-        <v>20190402</v>
-      </c>
+      <c r="N40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2393,9 +2315,7 @@
       <c r="M41" t="n">
         <v>353707.79</v>
       </c>
-      <c r="N41" t="n">
-        <v>20190408</v>
-      </c>
+      <c r="N41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2437,9 +2357,7 @@
       <c r="M42" t="n">
         <v>338027.79</v>
       </c>
-      <c r="N42" t="n">
-        <v>20190408</v>
-      </c>
+      <c r="N42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2485,9 +2403,7 @@
       <c r="M43" t="n">
         <v>328435.71</v>
       </c>
-      <c r="N43" t="n">
-        <v>20190408</v>
-      </c>
+      <c r="N43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2537,9 +2453,7 @@
       <c r="M44" t="n">
         <v>290906.3</v>
       </c>
-      <c r="N44" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2589,9 +2503,7 @@
       <c r="M45" t="n">
         <v>278663.4</v>
       </c>
-      <c r="N45" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2641,9 +2553,7 @@
       <c r="M46" t="n">
         <v>265219.28</v>
       </c>
-      <c r="N46" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2693,9 +2603,7 @@
       <c r="M47" t="n">
         <v>251865.16</v>
       </c>
-      <c r="N47" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2745,9 +2653,7 @@
       <c r="M48" t="n">
         <v>234358.09</v>
       </c>
-      <c r="N48" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2797,9 +2703,7 @@
       <c r="M49" t="n">
         <v>223759.84</v>
       </c>
-      <c r="N49" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2849,9 +2753,7 @@
       <c r="M50" t="n">
         <v>200448.24</v>
       </c>
-      <c r="N50" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2901,9 +2803,7 @@
       <c r="M51" t="n">
         <v>169770.89</v>
       </c>
-      <c r="N51" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2953,9 +2853,7 @@
       <c r="M52" t="n">
         <v>136213.54</v>
       </c>
-      <c r="N52" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -3005,9 +2903,7 @@
       <c r="M53" t="n">
         <v>108134.08</v>
       </c>
-      <c r="N53" t="n">
-        <v>20190410</v>
-      </c>
+      <c r="N53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3049,9 +2945,7 @@
       <c r="M54" t="n">
         <v>61542.08</v>
       </c>
-      <c r="N54" t="n">
-        <v>20190411</v>
-      </c>
+      <c r="N54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -3093,9 +2987,7 @@
       <c r="M55" t="n">
         <v>61492.08</v>
       </c>
-      <c r="N55" t="n">
-        <v>20190502</v>
-      </c>
+      <c r="N55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -3137,9 +3029,7 @@
       <c r="M56" t="n">
         <v>61454.84</v>
       </c>
-      <c r="N56" t="n">
-        <v>20190502</v>
-      </c>
+      <c r="N56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3181,9 +3071,7 @@
       <c r="M57" t="n">
         <v>61449.26</v>
       </c>
-      <c r="N57" t="n">
-        <v>20190502</v>
-      </c>
+      <c r="N57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3229,9 +3117,7 @@
       <c r="M58" t="n">
         <v>272513.26</v>
       </c>
-      <c r="N58" t="n">
-        <v>20190508</v>
-      </c>
+      <c r="N58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3281,9 +3167,7 @@
       <c r="M59" t="n">
         <v>472513.26</v>
       </c>
-      <c r="N59" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3325,9 +3209,7 @@
       <c r="M60" t="n">
         <v>454523.26</v>
       </c>
-      <c r="N60" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -3373,9 +3255,7 @@
       <c r="M61" t="n">
         <v>444494.67</v>
       </c>
-      <c r="N61" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3425,9 +3305,7 @@
       <c r="M62" t="n">
         <v>431050.54</v>
       </c>
-      <c r="N62" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3477,9 +3355,7 @@
       <c r="M63" t="n">
         <v>417696.41</v>
       </c>
-      <c r="N63" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3529,9 +3405,7 @@
       <c r="M64" t="n">
         <v>401405.23</v>
       </c>
-      <c r="N64" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3581,9 +3455,7 @@
       <c r="M65" t="n">
         <v>390806.98</v>
       </c>
-      <c r="N65" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3633,9 +3505,7 @@
       <c r="M66" t="n">
         <v>368755.73</v>
       </c>
-      <c r="N66" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -3685,9 +3555,7 @@
       <c r="M67" t="n">
         <v>339004.48</v>
       </c>
-      <c r="N67" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3737,9 +3605,7 @@
       <c r="M68" t="n">
         <v>306373.23</v>
       </c>
-      <c r="N68" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3789,9 +3655,7 @@
       <c r="M69" t="n">
         <v>280432.17</v>
       </c>
-      <c r="N69" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3841,9 +3705,7 @@
       <c r="M70" t="n">
         <v>270010.36</v>
       </c>
-      <c r="N70" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -3893,9 +3755,7 @@
       <c r="M71" t="n">
         <v>257767.46</v>
       </c>
-      <c r="N71" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3945,9 +3805,7 @@
       <c r="M72" t="n">
         <v>147434.13</v>
       </c>
-      <c r="N72" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3997,9 +3855,7 @@
       <c r="M73" t="n">
         <v>134343.13</v>
       </c>
-      <c r="N73" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -4049,9 +3905,7 @@
       <c r="M74" t="n">
         <v>94528.33</v>
       </c>
-      <c r="N74" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -4101,9 +3955,7 @@
       <c r="M75" t="n">
         <v>73548.33</v>
       </c>
-      <c r="N75" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -4153,9 +4005,7 @@
       <c r="M76" t="n">
         <v>70496.33</v>
       </c>
-      <c r="N76" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -4205,9 +4055,7 @@
       <c r="M77" t="n">
         <v>67076.33</v>
       </c>
-      <c r="N77" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -4257,9 +4105,7 @@
       <c r="M78" t="n">
         <v>64488.83</v>
       </c>
-      <c r="N78" t="n">
-        <v>20190510</v>
-      </c>
+      <c r="N78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -4301,9 +4147,7 @@
       <c r="M79" t="n">
         <v>11032.83</v>
       </c>
-      <c r="N79" t="n">
-        <v>20190513</v>
-      </c>
+      <c r="N79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -4353,9 +4197,7 @@
       <c r="M80" t="n">
         <v>7393.83</v>
       </c>
-      <c r="N80" t="n">
-        <v>20190520</v>
-      </c>
+      <c r="N80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -4405,9 +4247,7 @@
       <c r="M81" t="n">
         <v>6793.83</v>
       </c>
-      <c r="N81" t="n">
-        <v>20190520</v>
-      </c>
+      <c r="N81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -4457,9 +4297,7 @@
       <c r="M82" t="n">
         <v>56793.83</v>
       </c>
-      <c r="N82" t="n">
-        <v>20190523</v>
-      </c>
+      <c r="N82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -4509,9 +4347,7 @@
       <c r="M83" t="n">
         <v>106793.83</v>
       </c>
-      <c r="N83" t="n">
-        <v>20190523</v>
-      </c>
+      <c r="N83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -4561,9 +4397,7 @@
       <c r="M84" t="n">
         <v>76793.83</v>
       </c>
-      <c r="N84" t="n">
-        <v>20190523</v>
-      </c>
+      <c r="N84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -4613,9 +4447,7 @@
       <c r="M85" t="n">
         <v>46793.83</v>
       </c>
-      <c r="N85" t="n">
-        <v>20190523</v>
-      </c>
+      <c r="N85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -4665,9 +4497,7 @@
       <c r="M86" t="n">
         <v>49793.83</v>
       </c>
-      <c r="N86" t="n">
-        <v>20190524</v>
-      </c>
+      <c r="N86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -4717,9 +4547,7 @@
       <c r="M87" t="n">
         <v>484.31</v>
       </c>
-      <c r="N87" t="n">
-        <v>20190524</v>
-      </c>
+      <c r="N87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -4769,9 +4597,7 @@
       <c r="M88" t="n">
         <v>1200484.31</v>
       </c>
-      <c r="N88" t="n">
-        <v>20190529</v>
-      </c>
+      <c r="N88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -4821,9 +4647,7 @@
       <c r="M89" t="n">
         <v>1150484.31</v>
       </c>
-      <c r="N89" t="n">
-        <v>20190529</v>
-      </c>
+      <c r="N89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -4873,9 +4697,7 @@
       <c r="M90" t="n">
         <v>950484.3100000001</v>
       </c>
-      <c r="N90" t="n">
-        <v>20190529</v>
-      </c>
+      <c r="N90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -4925,9 +4747,7 @@
       <c r="M91" t="n">
         <v>850484.3100000001</v>
       </c>
-      <c r="N91" t="n">
-        <v>20190529</v>
-      </c>
+      <c r="N91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -4977,9 +4797,7 @@
       <c r="M92" t="n">
         <v>847484.3100000001</v>
       </c>
-      <c r="N92" t="n">
-        <v>20190529</v>
-      </c>
+      <c r="N92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -5021,9 +4839,7 @@
       <c r="M93" t="n">
         <v>847472.22</v>
       </c>
-      <c r="N93" t="n">
-        <v>20190602</v>
-      </c>
+      <c r="N93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -5065,9 +4881,7 @@
       <c r="M94" t="n">
         <v>847383.76</v>
       </c>
-      <c r="N94" t="n">
-        <v>20190602</v>
-      </c>
+      <c r="N94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -5109,9 +4923,7 @@
       <c r="M95" t="n">
         <v>847333.76</v>
       </c>
-      <c r="N95" t="n">
-        <v>20190602</v>
-      </c>
+      <c r="N95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -5157,9 +4969,7 @@
       <c r="M96" t="n">
         <v>826790.17</v>
       </c>
-      <c r="N96" t="n">
-        <v>20190604</v>
-      </c>
+      <c r="N96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -5201,9 +5011,7 @@
       <c r="M97" t="n">
         <v>808800.17</v>
       </c>
-      <c r="N97" t="n">
-        <v>20190605</v>
-      </c>
+      <c r="N97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -5253,9 +5061,7 @@
       <c r="M98" t="n">
         <v>797121.27</v>
       </c>
-      <c r="N98" t="n">
-        <v>20190606</v>
-      </c>
+      <c r="N98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -5305,9 +5111,7 @@
       <c r="M99" t="n">
         <v>740075.8199999999</v>
       </c>
-      <c r="N99" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -5357,9 +5161,7 @@
       <c r="M100" t="n">
         <v>726631.7</v>
       </c>
-      <c r="N100" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -5409,9 +5211,7 @@
       <c r="M101" t="n">
         <v>713771.95</v>
       </c>
-      <c r="N101" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -5461,9 +5261,7 @@
       <c r="M102" t="n">
         <v>697720.7</v>
       </c>
-      <c r="N102" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -5513,9 +5311,7 @@
       <c r="M103" t="n">
         <v>687122.45</v>
       </c>
-      <c r="N103" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -5565,9 +5361,7 @@
       <c r="M104" t="n">
         <v>665071.2</v>
       </c>
-      <c r="N104" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -5617,9 +5411,7 @@
       <c r="M105" t="n">
         <v>635319.95</v>
       </c>
-      <c r="N105" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -5669,9 +5461,7 @@
       <c r="M106" t="n">
         <v>602688.7</v>
       </c>
-      <c r="N106" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -5721,9 +5511,7 @@
       <c r="M107" t="n">
         <v>588364.5699999999</v>
       </c>
-      <c r="N107" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -5773,9 +5561,7 @@
       <c r="M108" t="n">
         <v>540454.5699999999</v>
       </c>
-      <c r="N108" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -5825,9 +5611,7 @@
       <c r="M109" t="n">
         <v>515234.57</v>
       </c>
-      <c r="N109" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -5877,9 +5661,7 @@
       <c r="M110" t="n">
         <v>479024.57</v>
       </c>
-      <c r="N110" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -5929,9 +5711,7 @@
       <c r="M111" t="n">
         <v>473667.62</v>
       </c>
-      <c r="N111" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -5981,9 +5761,7 @@
       <c r="M112" t="n">
         <v>454126.67</v>
       </c>
-      <c r="N112" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -6033,9 +5811,7 @@
       <c r="M113" t="n">
         <v>421617.67</v>
       </c>
-      <c r="N113" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -6085,9 +5861,7 @@
       <c r="M114" t="n">
         <v>421074.21</v>
       </c>
-      <c r="N114" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -6137,9 +5911,7 @@
       <c r="M115" t="n">
         <v>395133.15</v>
       </c>
-      <c r="N115" t="n">
-        <v>20190610</v>
-      </c>
+      <c r="N115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -6181,9 +5953,7 @@
       <c r="M116" t="n">
         <v>346740.05</v>
       </c>
-      <c r="N116" t="n">
-        <v>20190611</v>
-      </c>
+      <c r="N116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -6233,9 +6003,7 @@
       <c r="M117" t="n">
         <v>1846740.05</v>
       </c>
-      <c r="N117" t="n">
-        <v>20190612</v>
-      </c>
+      <c r="N117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -6285,9 +6053,7 @@
       <c r="M118" t="n">
         <v>246740.05</v>
       </c>
-      <c r="N118" t="n">
-        <v>20190620</v>
-      </c>
+      <c r="N118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -6329,9 +6095,7 @@
       <c r="M119" t="n">
         <v>246991.06</v>
       </c>
-      <c r="N119" t="n">
-        <v>20190621</v>
-      </c>
+      <c r="N119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -6381,9 +6145,7 @@
       <c r="M120" t="n">
         <v>143747.06</v>
       </c>
-      <c r="N120" t="n">
-        <v>20190625</v>
-      </c>
+      <c r="N120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -6429,9 +6191,7 @@
       <c r="M121" t="n">
         <v>173767.48</v>
       </c>
-      <c r="N121" t="n">
-        <v>20190627</v>
-      </c>
+      <c r="N121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -6481,9 +6241,7 @@
       <c r="M122" t="n">
         <v>85493.67</v>
       </c>
-      <c r="N122" t="n">
-        <v>20190628</v>
-      </c>
+      <c r="N122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -6533,9 +6291,7 @@
       <c r="M123" t="n">
         <v>8993.67</v>
       </c>
-      <c r="N123" t="n">
-        <v>20190628</v>
-      </c>
+      <c r="N123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -6577,9 +6333,7 @@
       <c r="M124" t="n">
         <v>8870.389999999999</v>
       </c>
-      <c r="N124" t="n">
-        <v>20190702</v>
-      </c>
+      <c r="N124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -6621,9 +6375,7 @@
       <c r="M125" t="n">
         <v>8861.09</v>
       </c>
-      <c r="N125" t="n">
-        <v>20190702</v>
-      </c>
+      <c r="N125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -6665,9 +6417,7 @@
       <c r="M126" t="n">
         <v>8811.09</v>
       </c>
-      <c r="N126" t="n">
-        <v>20190702</v>
-      </c>
+      <c r="N126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -6713,9 +6463,7 @@
       <c r="M127" t="n">
         <v>8529.18</v>
       </c>
-      <c r="N127" t="n">
-        <v>20190703</v>
-      </c>
+      <c r="N127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -6765,9 +6513,7 @@
       <c r="M128" t="n">
         <v>4929.18</v>
       </c>
-      <c r="N128" t="n">
-        <v>20190708</v>
-      </c>
+      <c r="N128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -6813,9 +6559,7 @@
       <c r="M129" t="n">
         <v>360550.43</v>
       </c>
-      <c r="N129" t="n">
-        <v>20190708</v>
-      </c>
+      <c r="N129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -6861,9 +6605,7 @@
       <c r="M130" t="n">
         <v>347045.24</v>
       </c>
-      <c r="N130" t="n">
-        <v>20190708</v>
-      </c>
+      <c r="N130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -6905,9 +6647,7 @@
       <c r="M131" t="n">
         <v>329055.24</v>
       </c>
-      <c r="N131" t="n">
-        <v>20190708</v>
-      </c>
+      <c r="N131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -6957,9 +6697,7 @@
       <c r="M132" t="n">
         <v>315611.11</v>
       </c>
-      <c r="N132" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -7009,9 +6747,7 @@
       <c r="M133" t="n">
         <v>304496.21</v>
       </c>
-      <c r="N133" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -7061,9 +6797,7 @@
       <c r="M134" t="n">
         <v>291744.96</v>
       </c>
-      <c r="N134" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -7113,9 +6847,7 @@
       <c r="M135" t="n">
         <v>275032.21</v>
       </c>
-      <c r="N135" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -7165,9 +6897,7 @@
       <c r="M136" t="n">
         <v>264433.96</v>
       </c>
-      <c r="N136" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -7217,9 +6947,7 @@
       <c r="M137" t="n">
         <v>241456.61</v>
       </c>
-      <c r="N137" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -7269,9 +6997,7 @@
       <c r="M138" t="n">
         <v>210779.26</v>
       </c>
-      <c r="N138" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -7321,9 +7047,7 @@
       <c r="M139" t="n">
         <v>179115.21</v>
       </c>
-      <c r="N139" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -7373,9 +7097,7 @@
       <c r="M140" t="n">
         <v>164791.09</v>
       </c>
-      <c r="N140" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -7425,9 +7147,7 @@
       <c r="M141" t="n">
         <v>136711.63</v>
       </c>
-      <c r="N141" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -7477,9 +7197,7 @@
       <c r="M142" t="n">
         <v>131780.63</v>
       </c>
-      <c r="N142" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -7529,9 +7247,7 @@
       <c r="M143" t="n">
         <v>88828.25</v>
       </c>
-      <c r="N143" t="n">
-        <v>20190710</v>
-      </c>
+      <c r="N143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -7573,9 +7289,7 @@
       <c r="M144" t="n">
         <v>40435.15</v>
       </c>
-      <c r="N144" t="n">
-        <v>20190711</v>
-      </c>
+      <c r="N144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -7625,9 +7339,7 @@
       <c r="M145" t="n">
         <v>32009.53</v>
       </c>
-      <c r="N145" t="n">
-        <v>20190712</v>
-      </c>
+      <c r="N145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -7677,9 +7389,7 @@
       <c r="M146" t="n">
         <v>30926.53</v>
       </c>
-      <c r="N146" t="n">
-        <v>20190712</v>
-      </c>
+      <c r="N146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -7729,9 +7439,7 @@
       <c r="M147" t="n">
         <v>19672.03</v>
       </c>
-      <c r="N147" t="n">
-        <v>20190712</v>
-      </c>
+      <c r="N147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -7781,9 +7489,7 @@
       <c r="M148" t="n">
         <v>9950.01</v>
       </c>
-      <c r="N148" t="n">
-        <v>20190717</v>
-      </c>
+      <c r="N148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -7829,9 +7535,7 @@
       <c r="M149" t="n">
         <v>9651.469999999999</v>
       </c>
-      <c r="N149" t="n">
-        <v>20190725</v>
-      </c>
+      <c r="N149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -7881,9 +7585,7 @@
       <c r="M150" t="n">
         <v>19094.47</v>
       </c>
-      <c r="N150" t="n">
-        <v>20190731</v>
-      </c>
+      <c r="N150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -7933,9 +7635,7 @@
       <c r="M151" t="n">
         <v>12799.14</v>
       </c>
-      <c r="N151" t="n">
-        <v>20190731</v>
-      </c>
+      <c r="N151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -7981,9 +7681,7 @@
       <c r="M152" t="n">
         <v>88105.39</v>
       </c>
-      <c r="N152" t="n">
-        <v>20190801</v>
-      </c>
+      <c r="N152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -8033,9 +7731,7 @@
       <c r="M153" t="n">
         <v>4158.02</v>
       </c>
-      <c r="N153" t="n">
-        <v>20190801</v>
-      </c>
+      <c r="N153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -8077,9 +7773,7 @@
       <c r="M154" t="n">
         <v>4097.3</v>
       </c>
-      <c r="N154" t="n">
-        <v>20190802</v>
-      </c>
+      <c r="N154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -8121,9 +7815,7 @@
       <c r="M155" t="n">
         <v>4089.86</v>
       </c>
-      <c r="N155" t="n">
-        <v>20190802</v>
-      </c>
+      <c r="N155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -8165,9 +7857,7 @@
       <c r="M156" t="n">
         <v>4039.86</v>
       </c>
-      <c r="N156" t="n">
-        <v>20190802</v>
-      </c>
+      <c r="N156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -8213,9 +7903,7 @@
       <c r="M157" t="n">
         <v>104496.8</v>
       </c>
-      <c r="N157" t="n">
-        <v>20190806</v>
-      </c>
+      <c r="N157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -8265,9 +7953,7 @@
       <c r="M158" t="n">
         <v>2736.8</v>
       </c>
-      <c r="N158" t="n">
-        <v>20190806</v>
-      </c>
+      <c r="N158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -8313,9 +7999,7 @@
       <c r="M159" t="n">
         <v>314243.74</v>
       </c>
-      <c r="N159" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -8365,9 +8049,7 @@
       <c r="M160" t="n">
         <v>302564.84</v>
       </c>
-      <c r="N160" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -8417,9 +8099,7 @@
       <c r="M161" t="n">
         <v>280941.34</v>
       </c>
-      <c r="N161" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -8469,9 +8149,7 @@
       <c r="M162" t="n">
         <v>277282.34</v>
       </c>
-      <c r="N162" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -8521,9 +8199,7 @@
       <c r="M163" t="n">
         <v>268608.34</v>
       </c>
-      <c r="N163" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -8573,9 +8249,7 @@
       <c r="M164" t="n">
         <v>268197.34</v>
       </c>
-      <c r="N164" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -8625,9 +8299,7 @@
       <c r="M165" t="n">
         <v>265197.34</v>
       </c>
-      <c r="N165" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -8669,9 +8341,7 @@
       <c r="M166" t="n">
         <v>92899.45</v>
       </c>
-      <c r="N166" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -8713,9 +8383,7 @@
       <c r="M167" t="n">
         <v>92894.95</v>
       </c>
-      <c r="N167" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -8757,9 +8425,7 @@
       <c r="M168" t="n">
         <v>74904.95</v>
       </c>
-      <c r="N168" t="n">
-        <v>20190809</v>
-      </c>
+      <c r="N168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -8805,9 +8471,7 @@
       <c r="M169" t="n">
         <v>58666.94</v>
       </c>
-      <c r="N169" t="n">
-        <v>20190812</v>
-      </c>
+      <c r="N169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -8849,9 +8513,7 @@
       <c r="M170" t="n">
         <v>10273.84</v>
       </c>
-      <c r="N170" t="n">
-        <v>20190813</v>
-      </c>
+      <c r="N170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -8901,9 +8563,7 @@
       <c r="M171" t="n">
         <v>20273.84</v>
       </c>
-      <c r="N171" t="n">
-        <v>20190814</v>
-      </c>
+      <c r="N171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -8949,9 +8609,7 @@
       <c r="M172" t="n">
         <v>30332.17</v>
       </c>
-      <c r="N172" t="n">
-        <v>20190819</v>
-      </c>
+      <c r="N172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -9001,9 +8659,7 @@
       <c r="M173" t="n">
         <v>5332.17</v>
       </c>
-      <c r="N173" t="n">
-        <v>20190820</v>
-      </c>
+      <c r="N173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -9049,9 +8705,7 @@
       <c r="M174" t="n">
         <v>161402.1</v>
       </c>
-      <c r="N174" t="n">
-        <v>20190830</v>
-      </c>
+      <c r="N174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -9101,9 +8755,7 @@
       <c r="M175" t="n">
         <v>79453.67</v>
       </c>
-      <c r="N175" t="n">
-        <v>20190830</v>
-      </c>
+      <c r="N175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -9153,9 +8805,7 @@
       <c r="M176" t="n">
         <v>2020.67</v>
       </c>
-      <c r="N176" t="n">
-        <v>20190830</v>
-      </c>
+      <c r="N176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -9197,9 +8847,7 @@
       <c r="M177" t="n">
         <v>1955.11</v>
       </c>
-      <c r="N177" t="n">
-        <v>20190902</v>
-      </c>
+      <c r="N177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -9241,9 +8889,7 @@
       <c r="M178" t="n">
         <v>1954.18</v>
       </c>
-      <c r="N178" t="n">
-        <v>20190902</v>
-      </c>
+      <c r="N178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -9285,9 +8931,7 @@
       <c r="M179" t="n">
         <v>1904.18</v>
       </c>
-      <c r="N179" t="n">
-        <v>20190902</v>
-      </c>
+      <c r="N179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -9333,9 +8977,7 @@
       <c r="M180" t="n">
         <v>27101.06</v>
       </c>
-      <c r="N180" t="n">
-        <v>20190909</v>
-      </c>
+      <c r="N180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -9385,9 +9027,7 @@
       <c r="M181" t="n">
         <v>2101.06</v>
       </c>
-      <c r="N181" t="n">
-        <v>20190909</v>
-      </c>
+      <c r="N181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -9433,9 +9073,7 @@
       <c r="M182" t="n">
         <v>329692.03</v>
       </c>
-      <c r="N182" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -9477,9 +9115,7 @@
       <c r="M183" t="n">
         <v>159220.88</v>
       </c>
-      <c r="N183" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -9521,9 +9157,7 @@
       <c r="M184" t="n">
         <v>159216.38</v>
       </c>
-      <c r="N184" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -9573,9 +9207,7 @@
       <c r="M185" t="n">
         <v>147311.88</v>
       </c>
-      <c r="N185" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -9625,9 +9257,7 @@
       <c r="M186" t="n">
         <v>131751.38</v>
       </c>
-      <c r="N186" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -9677,9 +9307,7 @@
       <c r="M187" t="n">
         <v>106570.88</v>
       </c>
-      <c r="N187" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -9729,9 +9357,7 @@
       <c r="M188" t="n">
         <v>102981.88</v>
       </c>
-      <c r="N188" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -9781,9 +9407,7 @@
       <c r="M189" t="n">
         <v>102769.98</v>
       </c>
-      <c r="N189" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -9833,9 +9457,7 @@
       <c r="M190" t="n">
         <v>100720.98</v>
       </c>
-      <c r="N190" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -9885,9 +9507,7 @@
       <c r="M191" t="n">
         <v>93068.06</v>
       </c>
-      <c r="N191" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -9937,9 +9557,7 @@
       <c r="M192" t="n">
         <v>90068.06</v>
       </c>
-      <c r="N192" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -9981,9 +9599,7 @@
       <c r="M193" t="n">
         <v>72078.06</v>
       </c>
-      <c r="N193" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -10029,9 +9645,7 @@
       <c r="M194" t="n">
         <v>54013.31</v>
       </c>
-      <c r="N194" t="n">
-        <v>20190910</v>
-      </c>
+      <c r="N194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -10073,9 +9687,7 @@
       <c r="M195" t="n">
         <v>5620.21</v>
       </c>
-      <c r="N195" t="n">
-        <v>20190911</v>
-      </c>
+      <c r="N195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -10121,9 +9733,7 @@
       <c r="M196" t="n">
         <v>20741.25</v>
       </c>
-      <c r="N196" t="n">
-        <v>20190911</v>
-      </c>
+      <c r="N196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -10173,9 +9783,7 @@
       <c r="M197" t="n">
         <v>741.25</v>
       </c>
-      <c r="N197" t="n">
-        <v>20190911</v>
-      </c>
+      <c r="N197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -10217,9 +9825,7 @@
       <c r="M198" t="n">
         <v>767.61</v>
       </c>
-      <c r="N198" t="n">
-        <v>20190921</v>
-      </c>
+      <c r="N198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -10265,9 +9871,7 @@
       <c r="M199" t="n">
         <v>177486.01</v>
       </c>
-      <c r="N199" t="n">
-        <v>20190929</v>
-      </c>
+      <c r="N199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -10317,9 +9921,7 @@
       <c r="M200" t="n">
         <v>81526.00999999999</v>
       </c>
-      <c r="N200" t="n">
-        <v>20190929</v>
-      </c>
+      <c r="N200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -10369,9 +9971,7 @@
       <c r="M201" t="n">
         <v>5206.01</v>
       </c>
-      <c r="N201" t="n">
-        <v>20190929</v>
-      </c>
+      <c r="N201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -10413,9 +10013,7 @@
       <c r="M202" t="n">
         <v>5205.08</v>
       </c>
-      <c r="N202" t="n">
-        <v>20191002</v>
-      </c>
+      <c r="N202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -10457,9 +10055,7 @@
       <c r="M203" t="n">
         <v>5162.8</v>
       </c>
-      <c r="N203" t="n">
-        <v>20191002</v>
-      </c>
+      <c r="N203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -10501,9 +10097,7 @@
       <c r="M204" t="n">
         <v>5112.8</v>
       </c>
-      <c r="N204" t="n">
-        <v>20191002</v>
-      </c>
+      <c r="N204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -10553,9 +10147,7 @@
       <c r="M205" t="n">
         <v>145112.8</v>
       </c>
-      <c r="N205" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -10605,9 +10197,7 @@
       <c r="M206" t="n">
         <v>295112.8</v>
       </c>
-      <c r="N206" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -10649,9 +10239,7 @@
       <c r="M207" t="n">
         <v>277122.8</v>
       </c>
-      <c r="N207" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -10697,9 +10285,7 @@
       <c r="M208" t="n">
         <v>257136.32</v>
       </c>
-      <c r="N208" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -10749,9 +10335,7 @@
       <c r="M209" t="n">
         <v>239636.32</v>
       </c>
-      <c r="N209" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -10801,9 +10385,7 @@
       <c r="M210" t="n">
         <v>227882.22</v>
       </c>
-      <c r="N210" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -10853,9 +10435,7 @@
       <c r="M211" t="n">
         <v>227282.22</v>
       </c>
-      <c r="N211" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -10897,9 +10477,7 @@
       <c r="M212" t="n">
         <v>52534.8</v>
       </c>
-      <c r="N212" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -10941,9 +10519,7 @@
       <c r="M213" t="n">
         <v>52530.3</v>
       </c>
-      <c r="N213" t="n">
-        <v>20191010</v>
-      </c>
+      <c r="N213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -10985,9 +10561,7 @@
       <c r="M214" t="n">
         <v>4137.2</v>
       </c>
-      <c r="N214" t="n">
-        <v>20191011</v>
-      </c>
+      <c r="N214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -11033,9 +10607,7 @@
       <c r="M215" t="n">
         <v>3451.65</v>
       </c>
-      <c r="N215" t="n">
-        <v>20191012</v>
-      </c>
+      <c r="N215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -11081,9 +10653,7 @@
       <c r="M216" t="n">
         <v>28743.32</v>
       </c>
-      <c r="N216" t="n">
-        <v>20191018</v>
-      </c>
+      <c r="N216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -11133,9 +10703,7 @@
       <c r="M217" t="n">
         <v>128743.32</v>
       </c>
-      <c r="N217" t="n">
-        <v>20191018</v>
-      </c>
+      <c r="N217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -11185,9 +10753,7 @@
       <c r="M218" t="n">
         <v>101543.32</v>
       </c>
-      <c r="N218" t="n">
-        <v>20191018</v>
-      </c>
+      <c r="N218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -11237,9 +10803,7 @@
       <c r="M219" t="n">
         <v>95272.32000000001</v>
       </c>
-      <c r="N219" t="n">
-        <v>20191018</v>
-      </c>
+      <c r="N219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -11289,9 +10853,7 @@
       <c r="M220" t="n">
         <v>33397.32</v>
       </c>
-      <c r="N220" t="n">
-        <v>20191024</v>
-      </c>
+      <c r="N220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -11341,9 +10903,7 @@
       <c r="M221" t="n">
         <v>233397.32</v>
       </c>
-      <c r="N221" t="n">
-        <v>20191030</v>
-      </c>
+      <c r="N221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -11393,9 +10953,7 @@
       <c r="M222" t="n">
         <v>155964.32</v>
       </c>
-      <c r="N222" t="n">
-        <v>20191030</v>
-      </c>
+      <c r="N222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -11445,9 +11003,7 @@
       <c r="M223" t="n">
         <v>61134.32</v>
       </c>
-      <c r="N223" t="n">
-        <v>20191030</v>
-      </c>
+      <c r="N223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -11497,9 +11053,7 @@
       <c r="M224" t="n">
         <v>151134.32</v>
       </c>
-      <c r="N224" t="n">
-        <v>20191030</v>
-      </c>
+      <c r="N224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -11549,9 +11103,7 @@
       <c r="M225" t="n">
         <v>1134.32</v>
       </c>
-      <c r="N225" t="n">
-        <v>20191030</v>
-      </c>
+      <c r="N225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -11601,9 +11153,7 @@
       <c r="M226" t="n">
         <v>24097.34</v>
       </c>
-      <c r="N226" t="n">
-        <v>20191101</v>
-      </c>
+      <c r="N226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -11645,9 +11195,7 @@
       <c r="M227" t="n">
         <v>24054.97</v>
       </c>
-      <c r="N227" t="n">
-        <v>20191102</v>
-      </c>
+      <c r="N227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -11689,9 +11237,7 @@
       <c r="M228" t="n">
         <v>24054.04</v>
       </c>
-      <c r="N228" t="n">
-        <v>20191102</v>
-      </c>
+      <c r="N228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -11733,9 +11279,7 @@
       <c r="M229" t="n">
         <v>24004.04</v>
       </c>
-      <c r="N229" t="n">
-        <v>20191102</v>
-      </c>
+      <c r="N229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -11777,9 +11321,7 @@
       <c r="M230" t="n">
         <v>24003.44</v>
       </c>
-      <c r="N230" t="n">
-        <v>20191103</v>
-      </c>
+      <c r="N230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -11829,9 +11371,7 @@
       <c r="M231" t="n">
         <v>8694.76</v>
       </c>
-      <c r="N231" t="n">
-        <v>20191106</v>
-      </c>
+      <c r="N231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -11877,9 +11417,7 @@
       <c r="M232" t="n">
         <v>38694.76</v>
       </c>
-      <c r="N232" t="n">
-        <v>20191107</v>
-      </c>
+      <c r="N232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -11929,9 +11467,7 @@
       <c r="M233" t="n">
         <v>238694.76</v>
       </c>
-      <c r="N233" t="n">
-        <v>20191108</v>
-      </c>
+      <c r="N233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -11981,9 +11517,7 @@
       <c r="M234" t="n">
         <v>226940.66</v>
       </c>
-      <c r="N234" t="n">
-        <v>20191108</v>
-      </c>
+      <c r="N234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -12025,9 +11559,7 @@
       <c r="M235" t="n">
         <v>95355.49000000001</v>
       </c>
-      <c r="N235" t="n">
-        <v>20191108</v>
-      </c>
+      <c r="N235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -12069,9 +11601,7 @@
       <c r="M236" t="n">
         <v>95351.49000000001</v>
       </c>
-      <c r="N236" t="n">
-        <v>20191108</v>
-      </c>
+      <c r="N236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -12113,9 +11643,7 @@
       <c r="M237" t="n">
         <v>79671.49000000001</v>
       </c>
-      <c r="N237" t="n">
-        <v>20191111</v>
-      </c>
+      <c r="N237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -12161,9 +11689,7 @@
       <c r="M238" t="n">
         <v>65893.25999999999</v>
       </c>
-      <c r="N238" t="n">
-        <v>20191111</v>
-      </c>
+      <c r="N238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -12213,9 +11739,7 @@
       <c r="M239" t="n">
         <v>55893.26</v>
       </c>
-      <c r="N239" t="n">
-        <v>20191111</v>
-      </c>
+      <c r="N239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -12257,9 +11781,7 @@
       <c r="M240" t="n">
         <v>13714.06</v>
       </c>
-      <c r="N240" t="n">
-        <v>20191112</v>
-      </c>
+      <c r="N240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -12309,9 +11831,7 @@
       <c r="M241" t="n">
         <v>93714.06</v>
       </c>
-      <c r="N241" t="n">
-        <v>20191118</v>
-      </c>
+      <c r="N241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -12361,9 +11881,7 @@
       <c r="M242" t="n">
         <v>17394.06</v>
       </c>
-      <c r="N242" t="n">
-        <v>20191118</v>
-      </c>
+      <c r="N242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -12413,9 +11931,7 @@
       <c r="M243" t="n">
         <v>14514.06</v>
       </c>
-      <c r="N243" t="n">
-        <v>20191120</v>
-      </c>
+      <c r="N243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -12457,9 +11973,7 @@
       <c r="M244" t="n">
         <v>14485.94</v>
       </c>
-      <c r="N244" t="n">
-        <v>20191202</v>
-      </c>
+      <c r="N244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -12501,9 +12015,7 @@
       <c r="M245" t="n">
         <v>14485.01</v>
       </c>
-      <c r="N245" t="n">
-        <v>20191202</v>
-      </c>
+      <c r="N245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -12545,9 +12057,7 @@
       <c r="M246" t="n">
         <v>14435.01</v>
       </c>
-      <c r="N246" t="n">
-        <v>20191202</v>
-      </c>
+      <c r="N246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -12597,9 +12107,7 @@
       <c r="M247" t="n">
         <v>113435.01</v>
       </c>
-      <c r="N247" t="n">
-        <v>20191202</v>
-      </c>
+      <c r="N247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -12649,9 +12157,7 @@
       <c r="M248" t="n">
         <v>14766.59</v>
       </c>
-      <c r="N248" t="n">
-        <v>20191202</v>
-      </c>
+      <c r="N248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -12701,9 +12207,7 @@
       <c r="M249" t="n">
         <v>12966.59</v>
       </c>
-      <c r="N249" t="n">
-        <v>20191203</v>
-      </c>
+      <c r="N249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -12753,9 +12257,7 @@
       <c r="M250" t="n">
         <v>247966.59</v>
       </c>
-      <c r="N250" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -12801,9 +12303,7 @@
       <c r="M251" t="n">
         <v>233650.06</v>
       </c>
-      <c r="N251" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -12845,9 +12345,7 @@
       <c r="M252" t="n">
         <v>217970.06</v>
       </c>
-      <c r="N252" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -12889,9 +12387,7 @@
       <c r="M253" t="n">
         <v>86203.19</v>
       </c>
-      <c r="N253" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -12933,9 +12429,7 @@
       <c r="M254" t="n">
         <v>86199.19</v>
       </c>
-      <c r="N254" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -12985,9 +12479,7 @@
       <c r="M255" t="n">
         <v>74445.09</v>
       </c>
-      <c r="N255" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -13037,9 +12529,7 @@
       <c r="M256" t="n">
         <v>60495.09</v>
       </c>
-      <c r="N256" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -13089,9 +12579,7 @@
       <c r="M257" t="n">
         <v>51513.81</v>
       </c>
-      <c r="N257" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -13141,9 +12629,7 @@
       <c r="M258" t="n">
         <v>49056.81</v>
       </c>
-      <c r="N258" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -13193,9 +12679,7 @@
       <c r="M259" t="n">
         <v>47816.81</v>
       </c>
-      <c r="N259" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -13245,9 +12729,7 @@
       <c r="M260" t="n">
         <v>46571.81</v>
       </c>
-      <c r="N260" t="n">
-        <v>20191210</v>
-      </c>
+      <c r="N260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -13289,9 +12771,7 @@
       <c r="M261" t="n">
         <v>4392.61</v>
       </c>
-      <c r="N261" t="n">
-        <v>20191211</v>
-      </c>
+      <c r="N261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -13341,9 +12821,7 @@
       <c r="M262" t="n">
         <v>2472.61</v>
       </c>
-      <c r="N262" t="n">
-        <v>20191212</v>
-      </c>
+      <c r="N262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -13385,9 +12863,7 @@
       <c r="M263" t="n">
         <v>2488.39</v>
       </c>
-      <c r="N263" t="n">
-        <v>20191221</v>
-      </c>
+      <c r="N263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -13437,9 +12913,7 @@
       <c r="M264" t="n">
         <v>142488.39</v>
       </c>
-      <c r="N264" t="n">
-        <v>20191227</v>
-      </c>
+      <c r="N264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -13489,9 +12963,7 @@
       <c r="M265" t="n">
         <v>42882.2</v>
       </c>
-      <c r="N265" t="n">
-        <v>20191227</v>
-      </c>
+      <c r="N265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -13541,9 +13013,7 @@
       <c r="M266" t="n">
         <v>42432.2</v>
       </c>
-      <c r="N266" t="n">
-        <v>20191227</v>
-      </c>
+      <c r="N266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -13585,9 +13055,7 @@
       <c r="M267" t="n">
         <v>42404.08</v>
       </c>
-      <c r="N267" t="n">
-        <v>20200102</v>
-      </c>
+      <c r="N267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -13629,9 +13097,7 @@
       <c r="M268" t="n">
         <v>42401.29</v>
       </c>
-      <c r="N268" t="n">
-        <v>20200102</v>
-      </c>
+      <c r="N268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -13673,9 +13139,7 @@
       <c r="M269" t="n">
         <v>42351.29</v>
       </c>
-      <c r="N269" t="n">
-        <v>20200102</v>
-      </c>
+      <c r="N269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -13721,9 +13185,7 @@
       <c r="M270" t="n">
         <v>40367.38</v>
       </c>
-      <c r="N270" t="n">
-        <v>20200106</v>
-      </c>
+      <c r="N270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -13773,9 +13235,7 @@
       <c r="M271" t="n">
         <v>230367.38</v>
       </c>
-      <c r="N271" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -13825,9 +13285,7 @@
       <c r="M272" t="n">
         <v>320367.38</v>
       </c>
-      <c r="N272" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -13869,9 +13327,7 @@
       <c r="M273" t="n">
         <v>184751.81</v>
       </c>
-      <c r="N273" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -13913,9 +13369,7 @@
       <c r="M274" t="n">
         <v>184747.81</v>
       </c>
-      <c r="N274" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -13965,9 +13419,7 @@
       <c r="M275" t="n">
         <v>172993.71</v>
       </c>
-      <c r="N275" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -14017,9 +13469,7 @@
       <c r="M276" t="n">
         <v>168673.71</v>
       </c>
-      <c r="N276" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -14069,9 +13519,7 @@
       <c r="M277" t="n">
         <v>132973.71</v>
       </c>
-      <c r="N277" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -14121,9 +13569,7 @@
       <c r="M278" t="n">
         <v>114547.75</v>
       </c>
-      <c r="N278" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -14173,9 +13619,7 @@
       <c r="M279" t="n">
         <v>112651.75</v>
       </c>
-      <c r="N279" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -14225,9 +13669,7 @@
       <c r="M280" t="n">
         <v>112301.95</v>
       </c>
-      <c r="N280" t="n">
-        <v>20200110</v>
-      </c>
+      <c r="N280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -14269,9 +13711,7 @@
       <c r="M281" t="n">
         <v>70122.75</v>
       </c>
-      <c r="N281" t="n">
-        <v>20200113</v>
-      </c>
+      <c r="N281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -14317,9 +13757,7 @@
       <c r="M282" t="n">
         <v>54845.92</v>
       </c>
-      <c r="N282" t="n">
-        <v>20200113</v>
-      </c>
+      <c r="N282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -14361,9 +13799,7 @@
       <c r="M283" t="n">
         <v>39165.92</v>
       </c>
-      <c r="N283" t="n">
-        <v>20200113</v>
-      </c>
+      <c r="N283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -14413,9 +13849,7 @@
       <c r="M284" t="n">
         <v>159165.92</v>
       </c>
-      <c r="N284" t="n">
-        <v>20200119</v>
-      </c>
+      <c r="N284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -14465,9 +13899,7 @@
       <c r="M285" t="n">
         <v>63005.92</v>
       </c>
-      <c r="N285" t="n">
-        <v>20200119</v>
-      </c>
+      <c r="N285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -14517,9 +13949,7 @@
       <c r="M286" t="n">
         <v>13005.92</v>
       </c>
-      <c r="N286" t="n">
-        <v>20200119</v>
-      </c>
+      <c r="N286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -14561,9 +13991,7 @@
       <c r="M287" t="n">
         <v>12973.05</v>
       </c>
-      <c r="N287" t="n">
-        <v>20200202</v>
-      </c>
+      <c r="N287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -14605,9 +14033,7 @@
       <c r="M288" t="n">
         <v>12971.19</v>
       </c>
-      <c r="N288" t="n">
-        <v>20200202</v>
-      </c>
+      <c r="N288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -14649,9 +14075,7 @@
       <c r="M289" t="n">
         <v>12921.19</v>
       </c>
-      <c r="N289" t="n">
-        <v>20200202</v>
-      </c>
+      <c r="N289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -14701,9 +14125,7 @@
       <c r="M290" t="n">
         <v>217921.19</v>
       </c>
-      <c r="N290" t="n">
-        <v>20200210</v>
-      </c>
+      <c r="N290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -14753,9 +14175,7 @@
       <c r="M291" t="n">
         <v>206167.09</v>
       </c>
-      <c r="N291" t="n">
-        <v>20200210</v>
-      </c>
+      <c r="N291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -14797,9 +14217,7 @@
       <c r="M292" t="n">
         <v>62997.13</v>
       </c>
-      <c r="N292" t="n">
-        <v>20200210</v>
-      </c>
+      <c r="N292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -14841,9 +14259,7 @@
       <c r="M293" t="n">
         <v>62993.13</v>
       </c>
-      <c r="N293" t="n">
-        <v>20200210</v>
-      </c>
+      <c r="N293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -14885,9 +14301,7 @@
       <c r="M294" t="n">
         <v>20813.93</v>
       </c>
-      <c r="N294" t="n">
-        <v>20200211</v>
-      </c>
+      <c r="N294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -14929,9 +14343,7 @@
       <c r="M295" t="n">
         <v>5133.93</v>
       </c>
-      <c r="N295" t="n">
-        <v>20200218</v>
-      </c>
+      <c r="N295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -14977,9 +14389,7 @@
       <c r="M296" t="n">
         <v>2580.49</v>
       </c>
-      <c r="N296" t="n">
-        <v>20200218</v>
-      </c>
+      <c r="N296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -15029,9 +14439,7 @@
       <c r="M297" t="n">
         <v>780.49</v>
       </c>
-      <c r="N297" t="n">
-        <v>20200227</v>
-      </c>
+      <c r="N297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -15081,9 +14489,7 @@
       <c r="M298" t="n">
         <v>97780.49000000001</v>
       </c>
-      <c r="N298" t="n">
-        <v>20200228</v>
-      </c>
+      <c r="N298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -15133,9 +14539,7 @@
       <c r="M299" t="n">
         <v>1033.43</v>
       </c>
-      <c r="N299" t="n">
-        <v>20200228</v>
-      </c>
+      <c r="N299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -15185,9 +14589,7 @@
       <c r="M300" t="n">
         <v>3033.43</v>
       </c>
-      <c r="N300" t="n">
-        <v>20200228</v>
-      </c>
+      <c r="N300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -15237,9 +14639,7 @@
       <c r="M301" t="n">
         <v>233.43</v>
       </c>
-      <c r="N301" t="n">
-        <v>20200228</v>
-      </c>
+      <c r="N301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -15281,9 +14681,7 @@
       <c r="M302" t="n">
         <v>214.8</v>
       </c>
-      <c r="N302" t="n">
-        <v>20200302</v>
-      </c>
+      <c r="N302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -15325,9 +14723,7 @@
       <c r="M303" t="n">
         <v>164.8</v>
       </c>
-      <c r="N303" t="n">
-        <v>20200302</v>
-      </c>
+      <c r="N303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -15369,9 +14765,7 @@
       <c r="M304" t="n">
         <v>164.2</v>
       </c>
-      <c r="N304" t="n">
-        <v>20200303</v>
-      </c>
+      <c r="N304" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
cross validation done and api setup
</commit_message>
<xml_diff>
--- a/Liushui/output/sample1.xlsx
+++ b/Liushui/output/sample1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -57,19 +57,87 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -14768,6 +14836,6 @@
       <c r="N304" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
option changed to option_list done
</commit_message>
<xml_diff>
--- a/Liushui/output/sample1.xlsx
+++ b/Liushui/output/sample1.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -505,7 +509,9 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" s="2" t="n">
+        <v>43831</v>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>2020-01-01 09:00:10</t>
@@ -543,13 +549,19 @@
       <c r="M2" t="n">
         <v>67227.7</v>
       </c>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>备用金</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" s="2" t="n">
+        <v>43832</v>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>2020-01-02 15:54:18</t>
@@ -587,13 +599,19 @@
       <c r="M3" t="n">
         <v>72527.7</v>
       </c>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" s="2" t="n">
+        <v>43832</v>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>2020-01-02 17:40:04</t>
@@ -631,13 +649,19 @@
       <c r="M4" t="n">
         <v>60557.7</v>
       </c>
-      <c r="N4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" s="2" t="n">
+        <v>43833</v>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>2020-01-03 16:04:25</t>
@@ -675,13 +699,19 @@
       <c r="M5" t="n">
         <v>53977.7</v>
       </c>
-      <c r="N5" t="inlineStr"/>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" s="2" t="n">
+        <v>43833</v>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>2020-01-03 16:04:26</t>
@@ -719,13 +749,19 @@
       <c r="M6" t="n">
         <v>51287.06</v>
       </c>
-      <c r="N6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" s="2" t="n">
+        <v>43833</v>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>2020-01-03 16:04:27</t>
@@ -763,13 +799,19 @@
       <c r="M7" t="n">
         <v>42287.06</v>
       </c>
-      <c r="N7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr"/>
+      <c r="B8" s="2" t="n">
+        <v>43834</v>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>2020-01-04 09:42:18</t>
@@ -807,13 +849,19 @@
       <c r="M8" t="n">
         <v>27693.14</v>
       </c>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>运费</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" s="2" t="n">
+        <v>43834</v>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>2020-01-04 09:42:20</t>
@@ -851,13 +899,19 @@
       <c r="M9" t="n">
         <v>25693.14</v>
       </c>
-      <c r="N9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>预支</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr"/>
+      <c r="B10" s="2" t="n">
+        <v>43836</v>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>2020-01-06 16:41:14</t>
@@ -895,13 +949,19 @@
       <c r="M10" t="n">
         <v>46693.14</v>
       </c>
-      <c r="N10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" s="2" t="n">
+        <v>43837</v>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>2020-01-07 17:07:54</t>
@@ -939,13 +999,19 @@
       <c r="M11" t="n">
         <v>46528.84</v>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr"/>
+      <c r="B12" s="2" t="n">
+        <v>43837</v>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>2020-01-07 17:17:54</t>
@@ -983,13 +1049,19 @@
       <c r="M12" t="n">
         <v>45228.84</v>
       </c>
-      <c r="N12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" s="2" t="n">
+        <v>43837</v>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t>2020-01-07 17:17:55</t>
@@ -1027,13 +1099,19 @@
       <c r="M13" t="n">
         <v>42228.84</v>
       </c>
-      <c r="N13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>预支</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" s="2" t="n">
+        <v>43837</v>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t>2020-01-07 17:17:56</t>
@@ -1071,13 +1149,19 @@
       <c r="M14" t="n">
         <v>41128.84</v>
       </c>
-      <c r="N14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr"/>
+      <c r="B15" s="2" t="n">
+        <v>43838</v>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t>2020-01-08 08:51:07</t>
@@ -1115,13 +1199,19 @@
       <c r="M15" t="n">
         <v>1391128.84</v>
       </c>
-      <c r="N15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>农行转泰隆</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr"/>
+      <c r="B16" s="2" t="n">
+        <v>43838</v>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t>2020-01-08 10:57:30</t>
@@ -1159,13 +1249,19 @@
       <c r="M16" t="n">
         <v>91128.84</v>
       </c>
-      <c r="N16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr"/>
+      <c r="B17" s="2" t="n">
+        <v>43838</v>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>2020-01-08 11:27:55</t>
@@ -1203,13 +1299,19 @@
       <c r="M17" t="n">
         <v>90848.84</v>
       </c>
-      <c r="N17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>年费</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr"/>
+      <c r="B18" s="2" t="n">
+        <v>43839</v>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t>2020-01-09 09:27:35</t>
@@ -1247,13 +1349,19 @@
       <c r="M18" t="n">
         <v>102648.84</v>
       </c>
-      <c r="N18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>材料费</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr"/>
+      <c r="B19" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t>2020-01-10 11:27:38</t>
@@ -1291,13 +1399,19 @@
       <c r="M19" t="n">
         <v>102517.04</v>
       </c>
-      <c r="N19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t>2020-01-10 16:12:43</t>
@@ -1335,13 +1449,19 @@
       <c r="M20" t="n">
         <v>95097.03999999999</v>
       </c>
-      <c r="N20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr"/>
+      <c r="B21" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>2020-01-10 16:12:44</t>
@@ -1379,13 +1499,19 @@
       <c r="M21" t="n">
         <v>80097.03999999999</v>
       </c>
-      <c r="N21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>泰隆转工行</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B22" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>2020-01-10 16:12:45</t>
@@ -1423,13 +1549,19 @@
       <c r="M22" t="n">
         <v>77340.35000000001</v>
       </c>
-      <c r="N22" t="inlineStr"/>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t>2020-01-10 16:12:47</t>
@@ -1467,13 +1599,19 @@
       <c r="M23" t="n">
         <v>75566.33</v>
       </c>
-      <c r="N23" t="inlineStr"/>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr"/>
+      <c r="B24" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t>2020-01-10 16:12:49</t>
@@ -1511,13 +1649,19 @@
       <c r="M24" t="n">
         <v>46166.33</v>
       </c>
-      <c r="N24" t="inlineStr"/>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr"/>
+      <c r="B25" s="2" t="n">
+        <v>43840</v>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t>2020-01-10 16:12:50</t>
@@ -1555,13 +1699,19 @@
       <c r="M25" t="n">
         <v>1766.33</v>
       </c>
-      <c r="N25" t="inlineStr"/>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t>2020-01-14 15:03:58</t>
@@ -1601,7 +1751,9 @@
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr"/>
+      <c r="B27" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t>2020-01-14 16:32:16</t>
@@ -1639,13 +1791,19 @@
       <c r="M27" t="n">
         <v>101625.56</v>
       </c>
-      <c r="N27" t="inlineStr"/>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr"/>
+      <c r="B28" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t>2020-01-14 16:58:24</t>
@@ -1683,13 +1841,19 @@
       <c r="M28" t="n">
         <v>100422.48</v>
       </c>
-      <c r="N28" t="inlineStr"/>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr"/>
+      <c r="B29" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t>2020-01-14 16:58:26</t>
@@ -1727,13 +1891,19 @@
       <c r="M29" t="n">
         <v>97635.48</v>
       </c>
-      <c r="N29" t="inlineStr"/>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr"/>
+      <c r="B30" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t>2020-01-14 16:58:27</t>
@@ -1771,13 +1941,19 @@
       <c r="M30" t="n">
         <v>87635.48</v>
       </c>
-      <c r="N30" t="inlineStr"/>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>咨询服务费</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr"/>
+      <c r="B31" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>2020-01-14 16:58:28</t>
@@ -1815,13 +1991,19 @@
       <c r="M31" t="n">
         <v>86335.48</v>
       </c>
-      <c r="N31" t="inlineStr"/>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr"/>
+      <c r="B32" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t>2020-01-14 16:58:30</t>
@@ -1859,13 +2041,19 @@
       <c r="M32" t="n">
         <v>84247.48</v>
       </c>
-      <c r="N32" t="inlineStr"/>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr"/>
+      <c r="B33" s="2" t="n">
+        <v>43844</v>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t>2020-01-14 16:58:31</t>
@@ -1903,13 +2091,19 @@
       <c r="M33" t="n">
         <v>82047.48</v>
       </c>
-      <c r="N33" t="inlineStr"/>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>广告制作费</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr"/>
+      <c r="B34" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t>2020-01-15 11:33:48</t>
@@ -1947,13 +2141,19 @@
       <c r="M34" t="n">
         <v>72810.84</v>
       </c>
-      <c r="N34" t="inlineStr"/>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr"/>
+      <c r="B35" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>2020-01-15 11:33:50</t>
@@ -1991,13 +2191,19 @@
       <c r="M35" t="n">
         <v>62287.85</v>
       </c>
-      <c r="N35" t="inlineStr"/>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr"/>
+      <c r="B36" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t>2020-01-15 15:16:39</t>
@@ -2035,13 +2241,19 @@
       <c r="M36" t="n">
         <v>65067.85</v>
       </c>
-      <c r="N36" t="inlineStr"/>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr"/>
+      <c r="B37" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C37" t="inlineStr">
         <is>
           <t>2020-01-15 16:19:58</t>
@@ -2081,7 +2293,9 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr"/>
+      <c r="B38" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C38" t="inlineStr">
         <is>
           <t>2020-01-15 16:56:07</t>
@@ -2119,13 +2333,19 @@
       <c r="M38" t="n">
         <v>364496.6</v>
       </c>
-      <c r="N38" t="inlineStr"/>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr"/>
+      <c r="B39" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>2020-01-15 16:56:09</t>
@@ -2163,13 +2383,19 @@
       <c r="M39" t="n">
         <v>364136.6</v>
       </c>
-      <c r="N39" t="inlineStr"/>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr"/>
+      <c r="B40" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C40" t="inlineStr">
         <is>
           <t>2020-01-15 16:56:10</t>
@@ -2207,13 +2433,19 @@
       <c r="M40" t="n">
         <v>363786.6</v>
       </c>
-      <c r="N40" t="inlineStr"/>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr"/>
+      <c r="B41" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>2020-01-15 16:56:11</t>
@@ -2251,13 +2483,19 @@
       <c r="M41" t="n">
         <v>363726.6</v>
       </c>
-      <c r="N41" t="inlineStr"/>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr"/>
+      <c r="B42" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C42" t="inlineStr">
         <is>
           <t>2020-01-15 21:56:24</t>
@@ -2295,13 +2533,19 @@
       <c r="M42" t="n">
         <v>362226.6</v>
       </c>
-      <c r="N42" t="inlineStr"/>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr"/>
+      <c r="B43" s="2" t="n">
+        <v>43845</v>
+      </c>
       <c r="C43" t="inlineStr">
         <is>
           <t>2020-01-15 21:56:25</t>
@@ -2339,13 +2583,19 @@
       <c r="M43" t="n">
         <v>348394.6</v>
       </c>
-      <c r="N43" t="inlineStr"/>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr"/>
+      <c r="B44" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C44" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:22</t>
@@ -2385,7 +2635,9 @@
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr"/>
+      <c r="B45" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C45" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:23</t>
@@ -2425,7 +2677,9 @@
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr"/>
+      <c r="B46" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C46" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:25</t>
@@ -2465,7 +2719,9 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr"/>
+      <c r="B47" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C47" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:26</t>
@@ -2505,7 +2761,9 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr"/>
+      <c r="B48" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C48" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:28</t>
@@ -2545,7 +2803,9 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr"/>
+      <c r="B49" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C49" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:29</t>
@@ -2585,7 +2845,9 @@
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr"/>
+      <c r="B50" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C50" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:31</t>
@@ -2625,7 +2887,9 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr"/>
+      <c r="B51" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C51" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:33</t>
@@ -2665,7 +2929,9 @@
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr"/>
+      <c r="B52" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C52" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:34</t>
@@ -2705,7 +2971,9 @@
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="inlineStr"/>
+      <c r="B53" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C53" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:36</t>
@@ -2745,7 +3013,9 @@
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="inlineStr"/>
+      <c r="B54" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C54" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:37</t>
@@ -2785,7 +3055,9 @@
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="inlineStr"/>
+      <c r="B55" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C55" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:39</t>
@@ -2825,7 +3097,9 @@
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="inlineStr"/>
+      <c r="B56" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C56" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:40</t>
@@ -2865,7 +3139,9 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr"/>
+      <c r="B57" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C57" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:42</t>
@@ -2905,7 +3181,9 @@
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="inlineStr"/>
+      <c r="B58" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C58" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:43</t>
@@ -2945,7 +3223,9 @@
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="inlineStr"/>
+      <c r="B59" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C59" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:45</t>
@@ -2985,7 +3265,9 @@
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr"/>
+      <c r="B60" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C60" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:46</t>
@@ -3025,7 +3307,9 @@
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61" t="inlineStr"/>
+      <c r="B61" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C61" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:48</t>
@@ -3065,7 +3349,9 @@
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr"/>
+      <c r="B62" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C62" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:49</t>
@@ -3105,7 +3391,9 @@
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr"/>
+      <c r="B63" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C63" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:51</t>
@@ -3145,7 +3433,9 @@
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr"/>
+      <c r="B64" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C64" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:52</t>
@@ -3185,7 +3475,9 @@
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="inlineStr"/>
+      <c r="B65" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C65" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:54</t>
@@ -3225,7 +3517,9 @@
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66" t="inlineStr"/>
+      <c r="B66" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C66" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:55</t>
@@ -3265,7 +3559,9 @@
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="inlineStr"/>
+      <c r="B67" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:57</t>
@@ -3305,7 +3601,9 @@
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="inlineStr"/>
+      <c r="B68" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C68" t="inlineStr">
         <is>
           <t>2020-01-16 22:04:58</t>
@@ -3345,7 +3643,9 @@
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="inlineStr"/>
+      <c r="B69" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:00</t>
@@ -3385,7 +3685,9 @@
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="inlineStr"/>
+      <c r="B70" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:01</t>
@@ -3425,7 +3727,9 @@
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71" t="inlineStr"/>
+      <c r="B71" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:03</t>
@@ -3465,7 +3769,9 @@
       <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72" t="inlineStr"/>
+      <c r="B72" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C72" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:05</t>
@@ -3505,7 +3811,9 @@
       <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B73" t="inlineStr"/>
+      <c r="B73" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C73" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:06</t>
@@ -3545,7 +3853,9 @@
       <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B74" t="inlineStr"/>
+      <c r="B74" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C74" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:08</t>
@@ -3585,7 +3895,9 @@
       <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B75" t="inlineStr"/>
+      <c r="B75" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C75" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:10</t>
@@ -3625,7 +3937,9 @@
       <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B76" t="inlineStr"/>
+      <c r="B76" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C76" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:11</t>
@@ -3665,7 +3979,9 @@
       <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B77" t="inlineStr"/>
+      <c r="B77" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C77" t="inlineStr">
         <is>
           <t>2020-01-16 22:05:12</t>
@@ -3705,7 +4021,9 @@
       <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78" t="inlineStr"/>
+      <c r="B78" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C78" t="inlineStr">
         <is>
           <t>2020-01-16 09:07:26</t>
@@ -3743,13 +4061,19 @@
       <c r="M78" t="n">
         <v>46352.14</v>
       </c>
-      <c r="N78" t="inlineStr"/>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79" t="inlineStr"/>
+      <c r="B79" s="2" t="n">
+        <v>43846</v>
+      </c>
       <c r="C79" t="inlineStr">
         <is>
           <t>2020-01-16 14:38:05</t>
@@ -3789,7 +4113,9 @@
       <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80" t="inlineStr"/>
+      <c r="B80" s="2" t="n">
+        <v>43847</v>
+      </c>
       <c r="C80" t="inlineStr">
         <is>
           <t>2020-01-17 16:38:18</t>
@@ -3827,13 +4153,19 @@
       <c r="M80" t="n">
         <v>148132.14</v>
       </c>
-      <c r="N80" t="inlineStr"/>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>定金</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="inlineStr"/>
+      <c r="B81" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C81" t="inlineStr">
         <is>
           <t>2020-01-19 15:37:58</t>
@@ -3871,13 +4203,19 @@
       <c r="M81" t="n">
         <v>147374.14</v>
       </c>
-      <c r="N81" t="inlineStr"/>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="inlineStr"/>
+      <c r="B82" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C82" t="inlineStr">
         <is>
           <t>2020-01-19 16:47:31</t>
@@ -3915,13 +4253,19 @@
       <c r="M82" t="n">
         <v>467374.14</v>
       </c>
-      <c r="N82" t="inlineStr"/>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>农行转泰隆</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83" t="inlineStr"/>
+      <c r="B83" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C83" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:35</t>
@@ -3959,13 +4303,19 @@
       <c r="M83" t="n">
         <v>464173.43</v>
       </c>
-      <c r="N83" t="inlineStr"/>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="inlineStr"/>
+      <c r="B84" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C84" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:36</t>
@@ -4003,13 +4353,19 @@
       <c r="M84" t="n">
         <v>462283.43</v>
       </c>
-      <c r="N84" t="inlineStr"/>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="inlineStr"/>
+      <c r="B85" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C85" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:38</t>
@@ -4047,13 +4403,19 @@
       <c r="M85" t="n">
         <v>458091.13</v>
       </c>
-      <c r="N85" t="inlineStr"/>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86" t="inlineStr"/>
+      <c r="B86" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C86" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:39</t>
@@ -4091,13 +4453,19 @@
       <c r="M86" t="n">
         <v>454211.13</v>
       </c>
-      <c r="N86" t="inlineStr"/>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>年终奖</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="inlineStr"/>
+      <c r="B87" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C87" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:42</t>
@@ -4135,13 +4503,19 @@
       <c r="M87" t="n">
         <v>452310.23</v>
       </c>
-      <c r="N87" t="inlineStr"/>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88" t="inlineStr"/>
+      <c r="B88" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C88" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:44</t>
@@ -4179,13 +4553,19 @@
       <c r="M88" t="n">
         <v>422603.18</v>
       </c>
-      <c r="N88" t="inlineStr"/>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>1-3月房租及12月电费</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89" t="inlineStr"/>
+      <c r="B89" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C89" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:53</t>
@@ -4223,13 +4603,19 @@
       <c r="M89" t="n">
         <v>412454.78</v>
       </c>
-      <c r="N89" t="inlineStr"/>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="inlineStr"/>
+      <c r="B90" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C90" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:54</t>
@@ -4267,13 +4653,19 @@
       <c r="M90" t="n">
         <v>398594.78</v>
       </c>
-      <c r="N90" t="inlineStr"/>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91" t="inlineStr"/>
+      <c r="B91" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C91" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:55</t>
@@ -4311,13 +4703,19 @@
       <c r="M91" t="n">
         <v>392048.82</v>
       </c>
-      <c r="N91" t="inlineStr"/>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92" t="inlineStr"/>
+      <c r="B92" s="2" t="n">
+        <v>43849</v>
+      </c>
       <c r="C92" t="inlineStr">
         <is>
           <t>2020-01-19 17:36:57</t>
@@ -4355,13 +4753,19 @@
       <c r="M92" t="n">
         <v>381119.82</v>
       </c>
-      <c r="N92" t="inlineStr"/>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="inlineStr"/>
+      <c r="B93" s="2" t="n">
+        <v>43850</v>
+      </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>2020-01-20 09:00:57</t>
@@ -4399,13 +4803,19 @@
       <c r="M93" t="n">
         <v>272062.32</v>
       </c>
-      <c r="N93" t="inlineStr"/>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="inlineStr"/>
+      <c r="B94" s="2" t="n">
+        <v>43850</v>
+      </c>
       <c r="C94" t="inlineStr">
         <is>
           <t>2020-01-20 09:03:55</t>
@@ -4443,13 +4853,19 @@
       <c r="M94" t="n">
         <v>221290.32</v>
       </c>
-      <c r="N94" t="inlineStr"/>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>运费</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95" t="inlineStr"/>
+      <c r="B95" s="2" t="n">
+        <v>43850</v>
+      </c>
       <c r="C95" t="inlineStr">
         <is>
           <t>2020-01-20 09:08:49</t>
@@ -4487,13 +4903,19 @@
       <c r="M95" t="n">
         <v>145670.32</v>
       </c>
-      <c r="N95" t="inlineStr"/>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96" t="inlineStr"/>
+      <c r="B96" s="2" t="n">
+        <v>43850</v>
+      </c>
       <c r="C96" t="inlineStr">
         <is>
           <t>2020-01-20 09:13:33</t>
@@ -4531,13 +4953,19 @@
       <c r="M96" t="n">
         <v>49932.82</v>
       </c>
-      <c r="N96" t="inlineStr"/>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97" t="inlineStr"/>
+      <c r="B97" s="2" t="n">
+        <v>43851</v>
+      </c>
       <c r="C97" t="inlineStr">
         <is>
           <t>2020-01-21 12:43:56</t>
@@ -4575,13 +5003,19 @@
       <c r="M97" t="n">
         <v>249932.82</v>
       </c>
-      <c r="N97" t="inlineStr"/>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>农行转泰隆</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98" t="inlineStr"/>
+      <c r="B98" s="2" t="n">
+        <v>43851</v>
+      </c>
       <c r="C98" t="inlineStr">
         <is>
           <t>2020-01-21 13:48:02</t>
@@ -4621,7 +5055,9 @@
       <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99" t="inlineStr"/>
+      <c r="B99" s="2" t="n">
+        <v>43851</v>
+      </c>
       <c r="C99" t="inlineStr">
         <is>
           <t>2020-01-21 13:48:19</t>
@@ -4659,13 +5095,19 @@
       <c r="M99" t="n">
         <v>50079.07</v>
       </c>
-      <c r="N99" t="inlineStr"/>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100" t="inlineStr"/>
+      <c r="B100" s="2" t="n">
+        <v>43880</v>
+      </c>
       <c r="C100" t="inlineStr">
         <is>
           <t>2020-02-19 09:57:55</t>
@@ -4703,13 +5145,19 @@
       <c r="M100" t="n">
         <v>50799.07</v>
       </c>
-      <c r="N100" t="inlineStr"/>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>货款，转浙江泰隆商业银行上海杨浦支行</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101" t="inlineStr"/>
+      <c r="B101" s="2" t="n">
+        <v>43880</v>
+      </c>
       <c r="C101" t="inlineStr">
         <is>
           <t>2020-02-19 11:26:45</t>
@@ -4747,13 +5195,19 @@
       <c r="M101" t="n">
         <v>52399.07</v>
       </c>
-      <c r="N101" t="inlineStr"/>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>无附言</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102" t="inlineStr"/>
+      <c r="B102" s="2" t="n">
+        <v>43881</v>
+      </c>
       <c r="C102" t="inlineStr">
         <is>
           <t>2020-02-20 15:36:12</t>
@@ -4791,13 +5245,19 @@
       <c r="M102" t="n">
         <v>68799.07000000001</v>
       </c>
-      <c r="N102" t="inlineStr"/>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103" t="inlineStr"/>
+      <c r="B103" s="2" t="n">
+        <v>43881</v>
+      </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>2020-02-20 15:46:55</t>
@@ -4835,13 +5295,19 @@
       <c r="M103" t="n">
         <v>63927.07</v>
       </c>
-      <c r="N103" t="inlineStr"/>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104" t="inlineStr"/>
+      <c r="B104" s="2" t="n">
+        <v>43881</v>
+      </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>2020-02-20 15:46:56</t>
@@ -4879,13 +5345,19 @@
       <c r="M104" t="n">
         <v>38426.07</v>
       </c>
-      <c r="N104" t="inlineStr"/>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105" t="inlineStr"/>
+      <c r="B105" s="2" t="n">
+        <v>43882</v>
+      </c>
       <c r="C105" t="inlineStr">
         <is>
           <t>2020-02-21 14:42:06</t>
@@ -4923,13 +5395,19 @@
       <c r="M105" t="n">
         <v>138426.07</v>
       </c>
-      <c r="N105" t="inlineStr"/>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>往来款</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106" t="inlineStr"/>
+      <c r="B106" s="2" t="n">
+        <v>43882</v>
+      </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>2020-02-21 14:46:27</t>
@@ -4969,7 +5447,9 @@
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107" t="inlineStr"/>
+      <c r="B107" s="2" t="n">
+        <v>43886</v>
+      </c>
       <c r="C107" t="inlineStr">
         <is>
           <t>2020-02-25 15:48:44</t>
@@ -5007,13 +5487,19 @@
       <c r="M107" t="n">
         <v>130426.07</v>
       </c>
-      <c r="N107" t="inlineStr"/>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108" t="inlineStr"/>
+      <c r="B108" s="2" t="n">
+        <v>43886</v>
+      </c>
       <c r="C108" t="inlineStr">
         <is>
           <t>2020-02-25 16:41:02</t>
@@ -5053,7 +5539,9 @@
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109" t="inlineStr"/>
+      <c r="B109" s="2" t="n">
+        <v>43886</v>
+      </c>
       <c r="C109" t="inlineStr">
         <is>
           <t>2020-02-25 17:08:29</t>
@@ -5093,7 +5581,9 @@
       <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="B110" t="inlineStr"/>
+      <c r="B110" s="2" t="n">
+        <v>43886</v>
+      </c>
       <c r="C110" t="inlineStr">
         <is>
           <t>2020-02-25 20:34:55</t>
@@ -5131,13 +5621,19 @@
       <c r="M110" t="n">
         <v>180563.07</v>
       </c>
-      <c r="N110" t="inlineStr"/>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>还款</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="B111" t="inlineStr"/>
+      <c r="B111" s="2" t="n">
+        <v>43886</v>
+      </c>
       <c r="C111" t="inlineStr">
         <is>
           <t>2020-02-25 20:35:13</t>
@@ -5177,7 +5673,9 @@
       <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="B112" t="inlineStr"/>
+      <c r="B112" s="2" t="n">
+        <v>43887</v>
+      </c>
       <c r="C112" t="inlineStr">
         <is>
           <t>2020-02-26 12:39:54</t>
@@ -5215,13 +5713,19 @@
       <c r="M112" t="n">
         <v>173046.64</v>
       </c>
-      <c r="N112" t="inlineStr"/>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B113" t="inlineStr"/>
+      <c r="B113" s="2" t="n">
+        <v>43887</v>
+      </c>
       <c r="C113" t="inlineStr">
         <is>
           <t>2020-02-26 15:42:51</t>
@@ -5261,7 +5765,9 @@
       <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="B114" t="inlineStr"/>
+      <c r="B114" s="2" t="n">
+        <v>43887</v>
+      </c>
       <c r="C114" t="inlineStr">
         <is>
           <t>2020-02-26 15:42:54</t>
@@ -5299,13 +5805,19 @@
       <c r="M114" t="n">
         <v>69646.64</v>
       </c>
-      <c r="N114" t="inlineStr"/>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>往来款</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="B115" t="inlineStr"/>
+      <c r="B115" s="2" t="n">
+        <v>43887</v>
+      </c>
       <c r="C115" t="inlineStr">
         <is>
           <t>2020-02-26 16:01:00</t>
@@ -5343,13 +5855,19 @@
       <c r="M115" t="n">
         <v>119646.64</v>
       </c>
-      <c r="N115" t="inlineStr"/>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>个人还款</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="B116" t="inlineStr"/>
+      <c r="B116" s="2" t="n">
+        <v>43888</v>
+      </c>
       <c r="C116" t="inlineStr">
         <is>
           <t>2020-02-27 17:08:24</t>
@@ -5387,13 +5905,19 @@
       <c r="M116" t="n">
         <v>119486.64</v>
       </c>
-      <c r="N116" t="inlineStr"/>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B117" t="inlineStr"/>
+      <c r="B117" s="2" t="n">
+        <v>43888</v>
+      </c>
       <c r="C117" t="inlineStr">
         <is>
           <t>2020-02-27 17:08:25</t>
@@ -5431,13 +5955,19 @@
       <c r="M117" t="n">
         <v>119406.64</v>
       </c>
-      <c r="N117" t="inlineStr"/>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>运费</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B118" t="inlineStr"/>
+      <c r="B118" s="2" t="n">
+        <v>43888</v>
+      </c>
       <c r="C118" t="inlineStr">
         <is>
           <t>2020-02-27 17:31:52</t>
@@ -5475,13 +6005,19 @@
       <c r="M118" t="n">
         <v>108906.64</v>
       </c>
-      <c r="N118" t="inlineStr"/>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="B119" t="inlineStr"/>
+      <c r="B119" s="2" t="n">
+        <v>43888</v>
+      </c>
       <c r="C119" t="inlineStr">
         <is>
           <t>2020-02-27 17:31:54</t>
@@ -5521,7 +6057,9 @@
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="B120" t="inlineStr"/>
+      <c r="B120" s="2" t="n">
+        <v>43888</v>
+      </c>
       <c r="C120" t="inlineStr">
         <is>
           <t>2020-02-27 17:31:56</t>
@@ -5559,13 +6097,19 @@
       <c r="M120" t="n">
         <v>101101.3</v>
       </c>
-      <c r="N120" t="inlineStr"/>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>预支</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="B121" t="inlineStr"/>
+      <c r="B121" s="2" t="n">
+        <v>43889</v>
+      </c>
       <c r="C121" t="inlineStr">
         <is>
           <t>2020-02-28 11:27:35</t>
@@ -5605,7 +6149,9 @@
       <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B122" t="inlineStr"/>
+      <c r="B122" s="2" t="n">
+        <v>43889</v>
+      </c>
       <c r="C122" t="inlineStr">
         <is>
           <t>2020-02-28 16:20:47</t>
@@ -5643,13 +6189,19 @@
       <c r="M122" t="n">
         <v>402057.55</v>
       </c>
-      <c r="N122" t="inlineStr"/>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>泰隆转农行</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B123" t="inlineStr"/>
+      <c r="B123" s="2" t="n">
+        <v>43889</v>
+      </c>
       <c r="C123" t="inlineStr">
         <is>
           <t>2020-02-28 16:20:48</t>
@@ -5687,13 +6239,19 @@
       <c r="M123" t="n">
         <v>364057.55</v>
       </c>
-      <c r="N123" t="inlineStr"/>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>往来款</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="B124" t="inlineStr"/>
+      <c r="B124" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C124" t="inlineStr">
         <is>
           <t>2020-03-01 18:17:32</t>
@@ -5731,13 +6289,19 @@
       <c r="M124" t="n">
         <v>814057.55</v>
       </c>
-      <c r="N124" t="inlineStr"/>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>还款</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125" t="inlineStr"/>
+      <c r="B125" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C125" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:29</t>
@@ -5777,7 +6341,9 @@
       <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="B126" t="inlineStr"/>
+      <c r="B126" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C126" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:30</t>
@@ -5817,7 +6383,9 @@
       <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="B127" t="inlineStr"/>
+      <c r="B127" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C127" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:31</t>
@@ -5857,7 +6425,9 @@
       <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="B128" t="inlineStr"/>
+      <c r="B128" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C128" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:33</t>
@@ -5897,7 +6467,9 @@
       <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="B129" t="inlineStr"/>
+      <c r="B129" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C129" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:34</t>
@@ -5937,7 +6509,9 @@
       <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="B130" t="inlineStr"/>
+      <c r="B130" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C130" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:35</t>
@@ -5977,7 +6551,9 @@
       <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="B131" t="inlineStr"/>
+      <c r="B131" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C131" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:37</t>
@@ -6017,7 +6593,9 @@
       <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="B132" t="inlineStr"/>
+      <c r="B132" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C132" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:38</t>
@@ -6057,7 +6635,9 @@
       <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="B133" t="inlineStr"/>
+      <c r="B133" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C133" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:39</t>
@@ -6097,7 +6677,9 @@
       <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="B134" t="inlineStr"/>
+      <c r="B134" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C134" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:41</t>
@@ -6137,7 +6719,9 @@
       <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="B135" t="inlineStr"/>
+      <c r="B135" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C135" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:42</t>
@@ -6177,7 +6761,9 @@
       <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="B136" t="inlineStr"/>
+      <c r="B136" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C136" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:44</t>
@@ -6217,7 +6803,9 @@
       <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="B137" t="inlineStr"/>
+      <c r="B137" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C137" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:46</t>
@@ -6257,7 +6845,9 @@
       <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="B138" t="inlineStr"/>
+      <c r="B138" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C138" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:47</t>
@@ -6297,7 +6887,9 @@
       <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="B139" t="inlineStr"/>
+      <c r="B139" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C139" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:49</t>
@@ -6337,7 +6929,9 @@
       <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="B140" t="inlineStr"/>
+      <c r="B140" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C140" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:50</t>
@@ -6377,7 +6971,9 @@
       <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="B141" t="inlineStr"/>
+      <c r="B141" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:51</t>
@@ -6417,7 +7013,9 @@
       <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="B142" t="inlineStr"/>
+      <c r="B142" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C142" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:53</t>
@@ -6457,7 +7055,9 @@
       <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="B143" t="inlineStr"/>
+      <c r="B143" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C143" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:54</t>
@@ -6497,7 +7097,9 @@
       <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="B144" t="inlineStr"/>
+      <c r="B144" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C144" t="inlineStr">
         <is>
           <t>2020-03-01 18:20:56</t>
@@ -6537,7 +7139,9 @@
       <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="B145" t="inlineStr"/>
+      <c r="B145" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C145" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:04</t>
@@ -6577,7 +7181,9 @@
       <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="B146" t="inlineStr"/>
+      <c r="B146" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C146" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:05</t>
@@ -6617,7 +7223,9 @@
       <c r="A147" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B147" t="inlineStr"/>
+      <c r="B147" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C147" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:07</t>
@@ -6657,7 +7265,9 @@
       <c r="A148" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="B148" t="inlineStr"/>
+      <c r="B148" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C148" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:09</t>
@@ -6697,7 +7307,9 @@
       <c r="A149" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="B149" t="inlineStr"/>
+      <c r="B149" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C149" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:11</t>
@@ -6737,7 +7349,9 @@
       <c r="A150" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="B150" t="inlineStr"/>
+      <c r="B150" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C150" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:12</t>
@@ -6777,7 +7391,9 @@
       <c r="A151" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="B151" t="inlineStr"/>
+      <c r="B151" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C151" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:13</t>
@@ -6817,7 +7433,9 @@
       <c r="A152" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B152" t="inlineStr"/>
+      <c r="B152" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C152" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:15</t>
@@ -6857,7 +7475,9 @@
       <c r="A153" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="B153" t="inlineStr"/>
+      <c r="B153" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C153" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:16</t>
@@ -6897,7 +7517,9 @@
       <c r="A154" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="B154" t="inlineStr"/>
+      <c r="B154" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C154" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:18</t>
@@ -6937,7 +7559,9 @@
       <c r="A155" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="B155" t="inlineStr"/>
+      <c r="B155" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C155" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:20</t>
@@ -6977,7 +7601,9 @@
       <c r="A156" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="B156" t="inlineStr"/>
+      <c r="B156" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C156" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:24</t>
@@ -7017,7 +7643,9 @@
       <c r="A157" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="B157" t="inlineStr"/>
+      <c r="B157" s="2" t="n">
+        <v>43891</v>
+      </c>
       <c r="C157" t="inlineStr">
         <is>
           <t>2020-03-01 18:21:26</t>
@@ -7057,7 +7685,9 @@
       <c r="A158" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="B158" t="inlineStr"/>
+      <c r="B158" s="2" t="n">
+        <v>43893</v>
+      </c>
       <c r="C158" t="inlineStr">
         <is>
           <t>2020-03-03 16:58:32</t>
@@ -7095,13 +7725,19 @@
       <c r="M158" t="n">
         <v>595302.85</v>
       </c>
-      <c r="N158" t="inlineStr"/>
+      <c r="N158" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="B159" t="inlineStr"/>
+      <c r="B159" s="2" t="n">
+        <v>43893</v>
+      </c>
       <c r="C159" t="inlineStr">
         <is>
           <t>2020-03-03 16:58:35</t>
@@ -7139,13 +7775,19 @@
       <c r="M159" t="n">
         <v>595227.85</v>
       </c>
-      <c r="N159" t="inlineStr"/>
+      <c r="N159" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="B160" t="inlineStr"/>
+      <c r="B160" s="2" t="n">
+        <v>43894</v>
+      </c>
       <c r="C160" t="inlineStr">
         <is>
           <t>2020-03-04 10:05:38</t>
@@ -7183,13 +7825,19 @@
       <c r="M160" t="n">
         <v>584276.5699999999</v>
       </c>
-      <c r="N160" t="inlineStr"/>
+      <c r="N160" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="B161" t="inlineStr"/>
+      <c r="B161" s="2" t="n">
+        <v>43894</v>
+      </c>
       <c r="C161" t="inlineStr">
         <is>
           <t>2020-03-04 10:05:40</t>
@@ -7227,13 +7875,19 @@
       <c r="M161" t="n">
         <v>538676.5699999999</v>
       </c>
-      <c r="N161" t="inlineStr"/>
+      <c r="N161" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="B162" t="inlineStr"/>
+      <c r="B162" s="2" t="n">
+        <v>43894</v>
+      </c>
       <c r="C162" t="inlineStr">
         <is>
           <t>2020-03-04 10:05:41</t>
@@ -7271,13 +7925,19 @@
       <c r="M162" t="n">
         <v>526576.5699999999</v>
       </c>
-      <c r="N162" t="inlineStr"/>
+      <c r="N162" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="B163" t="inlineStr"/>
+      <c r="B163" s="2" t="n">
+        <v>43894</v>
+      </c>
       <c r="C163" t="inlineStr">
         <is>
           <t>2020-03-04 17:50:56</t>
@@ -7315,13 +7975,19 @@
       <c r="M163" t="n">
         <v>526311.99</v>
       </c>
-      <c r="N163" t="inlineStr"/>
+      <c r="N163" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="B164" t="inlineStr"/>
+      <c r="B164" s="2" t="n">
+        <v>43894</v>
+      </c>
       <c r="C164" t="inlineStr">
         <is>
           <t>2020-03-04 17:50:57</t>
@@ -7359,13 +8025,19 @@
       <c r="M164" t="n">
         <v>525731.99</v>
       </c>
-      <c r="N164" t="inlineStr"/>
+      <c r="N164" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
         <v>163</v>
       </c>
-      <c r="B165" t="inlineStr"/>
+      <c r="B165" s="2" t="n">
+        <v>43894</v>
+      </c>
       <c r="C165" t="inlineStr">
         <is>
           <t>2020-03-04 17:50:59</t>
@@ -7403,13 +8075,19 @@
       <c r="M165" t="n">
         <v>525616.99</v>
       </c>
-      <c r="N165" t="inlineStr"/>
+      <c r="N165" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="B166" t="inlineStr"/>
+      <c r="B166" s="2" t="n">
+        <v>43895</v>
+      </c>
       <c r="C166" t="inlineStr">
         <is>
           <t>2020-03-05 10:32:50</t>
@@ -7447,13 +8125,19 @@
       <c r="M166" t="n">
         <v>275616.99</v>
       </c>
-      <c r="N166" t="inlineStr"/>
+      <c r="N166" t="inlineStr">
+        <is>
+          <t>泰隆转农行</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="B167" t="inlineStr"/>
+      <c r="B167" s="2" t="n">
+        <v>43896</v>
+      </c>
       <c r="C167" t="inlineStr">
         <is>
           <t>2020-03-06 16:32:29</t>
@@ -7491,13 +8175,19 @@
       <c r="M167" t="n">
         <v>274877.79</v>
       </c>
-      <c r="N167" t="inlineStr"/>
+      <c r="N167" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="B168" t="inlineStr"/>
+      <c r="B168" s="2" t="n">
+        <v>43896</v>
+      </c>
       <c r="C168" t="inlineStr">
         <is>
           <t>2020-03-06 17:25:18</t>
@@ -7535,13 +8225,19 @@
       <c r="M168" t="n">
         <v>233420.06</v>
       </c>
-      <c r="N168" t="inlineStr"/>
+      <c r="N168" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="B169" t="inlineStr"/>
+      <c r="B169" s="2" t="n">
+        <v>43897</v>
+      </c>
       <c r="C169" t="inlineStr">
         <is>
           <t>2020-03-07 09:00:30</t>
@@ -7579,13 +8275,19 @@
       <c r="M169" t="n">
         <v>154568.57</v>
       </c>
-      <c r="N169" t="inlineStr"/>
+      <c r="N169" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="B170" t="inlineStr"/>
+      <c r="B170" s="2" t="n">
+        <v>43899</v>
+      </c>
       <c r="C170" t="inlineStr">
         <is>
           <t>2020-03-09 20:48:17</t>
@@ -7623,13 +8325,19 @@
       <c r="M170" t="n">
         <v>147368.57</v>
       </c>
-      <c r="N170" t="inlineStr"/>
+      <c r="N170" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="B171" t="inlineStr"/>
+      <c r="B171" s="2" t="n">
+        <v>43899</v>
+      </c>
       <c r="C171" t="inlineStr">
         <is>
           <t>2020-03-09 20:48:18</t>
@@ -7667,13 +8375,19 @@
       <c r="M171" t="n">
         <v>140694.57</v>
       </c>
-      <c r="N171" t="inlineStr"/>
+      <c r="N171" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="B172" t="inlineStr"/>
+      <c r="B172" s="2" t="n">
+        <v>43899</v>
+      </c>
       <c r="C172" t="inlineStr">
         <is>
           <t>2020-03-09 20:48:19</t>
@@ -7711,13 +8425,19 @@
       <c r="M172" t="n">
         <v>136404.42</v>
       </c>
-      <c r="N172" t="inlineStr"/>
+      <c r="N172" t="inlineStr">
+        <is>
+          <t>运费</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
         <v>171</v>
       </c>
-      <c r="B173" t="inlineStr"/>
+      <c r="B173" s="2" t="n">
+        <v>43901</v>
+      </c>
       <c r="C173" t="inlineStr">
         <is>
           <t>2020-03-11 09:04:57</t>
@@ -7755,13 +8475,19 @@
       <c r="M173" t="n">
         <v>60679.42</v>
       </c>
-      <c r="N173" t="inlineStr"/>
+      <c r="N173" t="inlineStr">
+        <is>
+          <t>运费</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
         <v>172</v>
       </c>
-      <c r="B174" t="inlineStr"/>
+      <c r="B174" s="2" t="n">
+        <v>43901</v>
+      </c>
       <c r="C174" t="inlineStr">
         <is>
           <t>2020-03-11 11:13:14</t>
@@ -7799,13 +8525,19 @@
       <c r="M174" t="n">
         <v>70979.42</v>
       </c>
-      <c r="N174" t="inlineStr"/>
+      <c r="N174" t="inlineStr">
+        <is>
+          <t>公用动力驱动器</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="B175" t="inlineStr"/>
+      <c r="B175" s="2" t="n">
+        <v>43902</v>
+      </c>
       <c r="C175" t="inlineStr">
         <is>
           <t>2020-03-12 14:19:25</t>
@@ -7843,13 +8575,19 @@
       <c r="M175" t="n">
         <v>80979.42</v>
       </c>
-      <c r="N175" t="inlineStr"/>
+      <c r="N175" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="B176" t="inlineStr"/>
+      <c r="B176" s="2" t="n">
+        <v>43902</v>
+      </c>
       <c r="C176" t="inlineStr">
         <is>
           <t>2020-03-12 16:42:57</t>
@@ -7887,13 +8625,19 @@
       <c r="M176" t="n">
         <v>80229.42</v>
       </c>
-      <c r="N176" t="inlineStr"/>
+      <c r="N176" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="B177" t="inlineStr"/>
+      <c r="B177" s="2" t="n">
+        <v>43902</v>
+      </c>
       <c r="C177" t="inlineStr">
         <is>
           <t>2020-03-12 16:42:58</t>
@@ -7931,13 +8675,19 @@
       <c r="M177" t="n">
         <v>80129.42</v>
       </c>
-      <c r="N177" t="inlineStr"/>
+      <c r="N177" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
         <v>176</v>
       </c>
-      <c r="B178" t="inlineStr"/>
+      <c r="B178" s="2" t="n">
+        <v>43904</v>
+      </c>
       <c r="C178" t="inlineStr">
         <is>
           <t>2020-03-14 13:48:31</t>
@@ -7975,13 +8725,19 @@
       <c r="M178" t="n">
         <v>79729.42</v>
       </c>
-      <c r="N178" t="inlineStr"/>
+      <c r="N178" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="B179" t="inlineStr"/>
+      <c r="B179" s="2" t="n">
+        <v>43906</v>
+      </c>
       <c r="C179" t="inlineStr">
         <is>
           <t>2020-03-16 16:29:00</t>
@@ -8019,13 +8775,19 @@
       <c r="M179" t="n">
         <v>29729.42</v>
       </c>
-      <c r="N179" t="inlineStr"/>
+      <c r="N179" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
         <v>178</v>
       </c>
-      <c r="B180" t="inlineStr"/>
+      <c r="B180" s="2" t="n">
+        <v>43906</v>
+      </c>
       <c r="C180" t="inlineStr">
         <is>
           <t>2020-03-16 16:36:37</t>
@@ -8063,13 +8825,19 @@
       <c r="M180" t="n">
         <v>379729.42</v>
       </c>
-      <c r="N180" t="inlineStr"/>
+      <c r="N180" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="B181" t="inlineStr"/>
+      <c r="B181" s="2" t="n">
+        <v>43906</v>
+      </c>
       <c r="C181" t="inlineStr">
         <is>
           <t>2020-03-16 16:54:43</t>
@@ -8107,13 +8875,19 @@
       <c r="M181" t="n">
         <v>384829.42</v>
       </c>
-      <c r="N181" t="inlineStr"/>
+      <c r="N181" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="B182" t="inlineStr"/>
+      <c r="B182" s="2" t="n">
+        <v>43907</v>
+      </c>
       <c r="C182" t="inlineStr">
         <is>
           <t>2020-03-17 15:22:26</t>
@@ -8153,7 +8927,9 @@
       <c r="A183" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="B183" t="inlineStr"/>
+      <c r="B183" s="2" t="n">
+        <v>43907</v>
+      </c>
       <c r="C183" t="inlineStr">
         <is>
           <t>2020-03-17 17:22:27</t>
@@ -8191,13 +8967,19 @@
       <c r="M183" t="n">
         <v>829229.42</v>
       </c>
-      <c r="N183" t="inlineStr"/>
+      <c r="N183" t="inlineStr">
+        <is>
+          <t>往来款</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
         <v>182</v>
       </c>
-      <c r="B184" t="inlineStr"/>
+      <c r="B184" s="2" t="n">
+        <v>43907</v>
+      </c>
       <c r="C184" t="inlineStr">
         <is>
           <t>2020-03-17 17:29:10</t>
@@ -8235,13 +9017,19 @@
       <c r="M184" t="n">
         <v>279229.42</v>
       </c>
-      <c r="N184" t="inlineStr"/>
+      <c r="N184" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="B185" t="inlineStr"/>
+      <c r="B185" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C185" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:01</t>
@@ -8279,13 +9067,19 @@
       <c r="M185" t="n">
         <v>245999.65</v>
       </c>
-      <c r="N185" t="inlineStr"/>
+      <c r="N185" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
         <v>184</v>
       </c>
-      <c r="B186" t="inlineStr"/>
+      <c r="B186" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C186" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:02</t>
@@ -8323,13 +9117,19 @@
       <c r="M186" t="n">
         <v>240803.37</v>
       </c>
-      <c r="N186" t="inlineStr"/>
+      <c r="N186" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="B187" t="inlineStr"/>
+      <c r="B187" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C187" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:04</t>
@@ -8367,13 +9167,19 @@
       <c r="M187" t="n">
         <v>235801.02</v>
       </c>
-      <c r="N187" t="inlineStr"/>
+      <c r="N187" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
         <v>186</v>
       </c>
-      <c r="B188" t="inlineStr"/>
+      <c r="B188" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C188" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:06</t>
@@ -8411,13 +9217,19 @@
       <c r="M188" t="n">
         <v>230216.74</v>
       </c>
-      <c r="N188" t="inlineStr"/>
+      <c r="N188" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="B189" t="inlineStr"/>
+      <c r="B189" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C189" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:08</t>
@@ -8455,13 +9267,19 @@
       <c r="M189" t="n">
         <v>225668.04</v>
       </c>
-      <c r="N189" t="inlineStr"/>
+      <c r="N189" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="B190" t="inlineStr"/>
+      <c r="B190" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C190" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:09</t>
@@ -8499,13 +9317,19 @@
       <c r="M190" t="n">
         <v>222405.69</v>
       </c>
-      <c r="N190" t="inlineStr"/>
+      <c r="N190" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
         <v>189</v>
       </c>
-      <c r="B191" t="inlineStr"/>
+      <c r="B191" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C191" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:11</t>
@@ -8543,13 +9367,19 @@
       <c r="M191" t="n">
         <v>207405.69</v>
       </c>
-      <c r="N191" t="inlineStr"/>
+      <c r="N191" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="B192" t="inlineStr"/>
+      <c r="B192" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C192" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:12</t>
@@ -8587,13 +9417,19 @@
       <c r="M192" t="n">
         <v>192405.69</v>
       </c>
-      <c r="N192" t="inlineStr"/>
+      <c r="N192" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
         <v>191</v>
       </c>
-      <c r="B193" t="inlineStr"/>
+      <c r="B193" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C193" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:14</t>
@@ -8631,13 +9467,19 @@
       <c r="M193" t="n">
         <v>182280.14</v>
       </c>
-      <c r="N193" t="inlineStr"/>
+      <c r="N193" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="B194" t="inlineStr"/>
+      <c r="B194" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C194" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:16</t>
@@ -8675,13 +9517,19 @@
       <c r="M194" t="n">
         <v>174665.88</v>
       </c>
-      <c r="N194" t="inlineStr"/>
+      <c r="N194" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
         <v>193</v>
       </c>
-      <c r="B195" t="inlineStr"/>
+      <c r="B195" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C195" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:17</t>
@@ -8719,13 +9567,19 @@
       <c r="M195" t="n">
         <v>169794.06</v>
       </c>
-      <c r="N195" t="inlineStr"/>
+      <c r="N195" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
         <v>194</v>
       </c>
-      <c r="B196" t="inlineStr"/>
+      <c r="B196" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C196" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:19</t>
@@ -8763,13 +9617,19 @@
       <c r="M196" t="n">
         <v>167528.06</v>
       </c>
-      <c r="N196" t="inlineStr"/>
+      <c r="N196" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="B197" t="inlineStr"/>
+      <c r="B197" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C197" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:21</t>
@@ -8807,13 +9667,19 @@
       <c r="M197" t="n">
         <v>163528.06</v>
       </c>
-      <c r="N197" t="inlineStr"/>
+      <c r="N197" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
         <v>196</v>
       </c>
-      <c r="B198" t="inlineStr"/>
+      <c r="B198" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C198" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:23</t>
@@ -8851,13 +9717,19 @@
       <c r="M198" t="n">
         <v>155618.06</v>
       </c>
-      <c r="N198" t="inlineStr"/>
+      <c r="N198" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
         <v>197</v>
       </c>
-      <c r="B199" t="inlineStr"/>
+      <c r="B199" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C199" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:24</t>
@@ -8895,13 +9767,19 @@
       <c r="M199" t="n">
         <v>147708.06</v>
       </c>
-      <c r="N199" t="inlineStr"/>
+      <c r="N199" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
         <v>198</v>
       </c>
-      <c r="B200" t="inlineStr"/>
+      <c r="B200" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C200" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:26</t>
@@ -8939,13 +9817,19 @@
       <c r="M200" t="n">
         <v>139798.06</v>
       </c>
-      <c r="N200" t="inlineStr"/>
+      <c r="N200" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="B201" t="inlineStr"/>
+      <c r="B201" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C201" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:28</t>
@@ -8983,13 +9867,19 @@
       <c r="M201" t="n">
         <v>136740.71</v>
       </c>
-      <c r="N201" t="inlineStr"/>
+      <c r="N201" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="B202" t="inlineStr"/>
+      <c r="B202" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C202" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:29</t>
@@ -9027,13 +9917,19 @@
       <c r="M202" t="n">
         <v>134638.36</v>
       </c>
-      <c r="N202" t="inlineStr"/>
+      <c r="N202" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="B203" t="inlineStr"/>
+      <c r="B203" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C203" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:31</t>
@@ -9071,13 +9967,19 @@
       <c r="M203" t="n">
         <v>120612.46</v>
       </c>
-      <c r="N203" t="inlineStr"/>
+      <c r="N203" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
         <v>202</v>
       </c>
-      <c r="B204" t="inlineStr"/>
+      <c r="B204" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C204" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:33</t>
@@ -9115,13 +10017,19 @@
       <c r="M204" t="n">
         <v>117556.11</v>
       </c>
-      <c r="N204" t="inlineStr"/>
+      <c r="N204" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
         <v>203</v>
       </c>
-      <c r="B205" t="inlineStr"/>
+      <c r="B205" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C205" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:35</t>
@@ -9159,13 +10067,19 @@
       <c r="M205" t="n">
         <v>114953.76</v>
       </c>
-      <c r="N205" t="inlineStr"/>
+      <c r="N205" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
         <v>204</v>
       </c>
-      <c r="B206" t="inlineStr"/>
+      <c r="B206" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C206" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:36</t>
@@ -9203,13 +10117,19 @@
       <c r="M206" t="n">
         <v>112081.41</v>
       </c>
-      <c r="N206" t="inlineStr"/>
+      <c r="N206" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
         <v>205</v>
       </c>
-      <c r="B207" t="inlineStr"/>
+      <c r="B207" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C207" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:38</t>
@@ -9247,13 +10167,19 @@
       <c r="M207" t="n">
         <v>108611.3</v>
       </c>
-      <c r="N207" t="inlineStr"/>
+      <c r="N207" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="B208" t="inlineStr"/>
+      <c r="B208" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C208" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:39</t>
@@ -9291,13 +10217,19 @@
       <c r="M208" t="n">
         <v>105611.3</v>
       </c>
-      <c r="N208" t="inlineStr"/>
+      <c r="N208" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
         <v>207</v>
       </c>
-      <c r="B209" t="inlineStr"/>
+      <c r="B209" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C209" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:41</t>
@@ -9335,13 +10267,19 @@
       <c r="M209" t="n">
         <v>101108.95</v>
       </c>
-      <c r="N209" t="inlineStr"/>
+      <c r="N209" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="B210" t="inlineStr"/>
+      <c r="B210" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C210" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:42</t>
@@ -9379,13 +10317,19 @@
       <c r="M210" t="n">
         <v>97106.60000000001</v>
       </c>
-      <c r="N210" t="inlineStr"/>
+      <c r="N210" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
         <v>209</v>
       </c>
-      <c r="B211" t="inlineStr"/>
+      <c r="B211" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C211" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:44</t>
@@ -9423,13 +10367,19 @@
       <c r="M211" t="n">
         <v>92790.25</v>
       </c>
-      <c r="N211" t="inlineStr"/>
+      <c r="N211" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
         <v>210</v>
       </c>
-      <c r="B212" t="inlineStr"/>
+      <c r="B212" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C212" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:45</t>
@@ -9467,13 +10417,19 @@
       <c r="M212" t="n">
         <v>87424.25</v>
       </c>
-      <c r="N212" t="inlineStr"/>
+      <c r="N212" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
         <v>211</v>
       </c>
-      <c r="B213" t="inlineStr"/>
+      <c r="B213" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C213" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:47</t>
@@ -9511,13 +10467,19 @@
       <c r="M213" t="n">
         <v>82560.95</v>
       </c>
-      <c r="N213" t="inlineStr"/>
+      <c r="N213" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="B214" t="inlineStr"/>
+      <c r="B214" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C214" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:48</t>
@@ -9555,13 +10517,19 @@
       <c r="M214" t="n">
         <v>79344.60000000001</v>
       </c>
-      <c r="N214" t="inlineStr"/>
+      <c r="N214" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
         <v>213</v>
       </c>
-      <c r="B215" t="inlineStr"/>
+      <c r="B215" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C215" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:50</t>
@@ -9599,13 +10567,19 @@
       <c r="M215" t="n">
         <v>74286.78</v>
       </c>
-      <c r="N215" t="inlineStr"/>
+      <c r="N215" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="B216" t="inlineStr"/>
+      <c r="B216" s="2" t="n">
+        <v>43908</v>
+      </c>
       <c r="C216" t="inlineStr">
         <is>
           <t>2020-03-18 16:50:52</t>
@@ -9643,13 +10617,19 @@
       <c r="M216" t="n">
         <v>69720.78</v>
       </c>
-      <c r="N216" t="inlineStr"/>
+      <c r="N216" t="inlineStr">
+        <is>
+          <t>工资</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
         <v>215</v>
       </c>
-      <c r="B217" t="inlineStr"/>
+      <c r="B217" s="2" t="n">
+        <v>43909</v>
+      </c>
       <c r="C217" t="inlineStr">
         <is>
           <t>2020-03-19 09:34:49</t>
@@ -9689,7 +10669,9 @@
       <c r="A218" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="B218" t="inlineStr"/>
+      <c r="B218" s="2" t="n">
+        <v>43909</v>
+      </c>
       <c r="C218" t="inlineStr">
         <is>
           <t>2020-03-19 14:38:43</t>
@@ -9727,13 +10709,19 @@
       <c r="M218" t="n">
         <v>618245.22</v>
       </c>
-      <c r="N218" t="inlineStr"/>
+      <c r="N218" t="inlineStr">
+        <is>
+          <t>预支</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
         <v>217</v>
       </c>
-      <c r="B219" t="inlineStr"/>
+      <c r="B219" s="2" t="n">
+        <v>43909</v>
+      </c>
       <c r="C219" t="inlineStr">
         <is>
           <t>2020-03-19 14:38:44</t>
@@ -9771,13 +10759,19 @@
       <c r="M219" t="n">
         <v>547803.61</v>
       </c>
-      <c r="N219" t="inlineStr"/>
+      <c r="N219" t="inlineStr">
+        <is>
+          <t>运费</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="B220" t="inlineStr"/>
+      <c r="B220" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C220" t="inlineStr">
         <is>
           <t>2020-03-20 09:45:11</t>
@@ -9815,13 +10809,19 @@
       <c r="M220" t="n">
         <v>47803.61</v>
       </c>
-      <c r="N220" t="inlineStr"/>
+      <c r="N220" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
         <v>219</v>
       </c>
-      <c r="B221" t="inlineStr"/>
+      <c r="B221" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C221" t="inlineStr">
         <is>
           <t>2020-03-20 09:53:01</t>
@@ -9859,13 +10859,19 @@
       <c r="M221" t="n">
         <v>49303.61</v>
       </c>
-      <c r="N221" t="inlineStr"/>
+      <c r="N221" t="inlineStr">
+        <is>
+          <t>账户已销户或账户不存在</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="B222" t="inlineStr"/>
+      <c r="B222" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C222" t="inlineStr">
         <is>
           <t>2020-03-20 14:31:52</t>
@@ -9903,13 +10909,19 @@
       <c r="M222" t="n">
         <v>51053.61</v>
       </c>
-      <c r="N222" t="inlineStr"/>
+      <c r="N222" t="inlineStr">
+        <is>
+          <t>尾款</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
         <v>221</v>
       </c>
-      <c r="B223" t="inlineStr"/>
+      <c r="B223" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C223" t="inlineStr">
         <is>
           <t>2020-03-20 15:58:41</t>
@@ -9947,13 +10959,19 @@
       <c r="M223" t="n">
         <v>4933.61</v>
       </c>
-      <c r="N223" t="inlineStr"/>
+      <c r="N223" t="inlineStr">
+        <is>
+          <t>材料费</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="B224" t="inlineStr"/>
+      <c r="B224" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C224" t="inlineStr">
         <is>
           <t>2020-03-20 15:58:42</t>
@@ -9991,13 +11009,19 @@
       <c r="M224" t="n">
         <v>3433.61</v>
       </c>
-      <c r="N224" t="inlineStr"/>
+      <c r="N224" t="inlineStr">
+        <is>
+          <t>预支</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="B225" t="inlineStr"/>
+      <c r="B225" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C225" t="inlineStr">
         <is>
           <t>2020-03-20 17:10:29</t>
@@ -10037,7 +11061,9 @@
       <c r="A226" s="1" t="n">
         <v>224</v>
       </c>
-      <c r="B226" t="inlineStr"/>
+      <c r="B226" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C226" t="inlineStr">
         <is>
           <t>2020-03-20 17:28:40</t>
@@ -10075,13 +11101,19 @@
       <c r="M226" t="n">
         <v>503052.21</v>
       </c>
-      <c r="N226" t="inlineStr"/>
+      <c r="N226" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="B227" t="inlineStr"/>
+      <c r="B227" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C227" t="inlineStr">
         <is>
           <t>2020-03-20 17:28:41</t>
@@ -10119,13 +11151,19 @@
       <c r="M227" t="n">
         <v>502840.21</v>
       </c>
-      <c r="N227" t="inlineStr"/>
+      <c r="N227" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="B228" t="inlineStr"/>
+      <c r="B228" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C228" t="inlineStr">
         <is>
           <t>2020-03-20 17:28:42</t>
@@ -10163,13 +11201,19 @@
       <c r="M228" t="n">
         <v>501952.21</v>
       </c>
-      <c r="N228" t="inlineStr"/>
+      <c r="N228" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="B229" t="inlineStr"/>
+      <c r="B229" s="2" t="n">
+        <v>43910</v>
+      </c>
       <c r="C229" t="inlineStr">
         <is>
           <t>2020-03-20 17:35:35</t>
@@ -10207,13 +11251,19 @@
       <c r="M229" t="n">
         <v>451952.21</v>
       </c>
-      <c r="N229" t="inlineStr"/>
+      <c r="N229" t="inlineStr">
+        <is>
+          <t>保证金</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
         <v>228</v>
       </c>
-      <c r="B230" t="inlineStr"/>
+      <c r="B230" s="2" t="n">
+        <v>43911</v>
+      </c>
       <c r="C230" t="inlineStr">
         <is>
           <t>2020-03-21 00:38:20</t>
@@ -10253,7 +11303,9 @@
       <c r="A231" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="B231" t="inlineStr"/>
+      <c r="B231" s="2" t="n">
+        <v>43911</v>
+      </c>
       <c r="C231" t="inlineStr">
         <is>
           <t>2020-03-21 09:30:16</t>
@@ -10291,13 +11343,19 @@
       <c r="M231" t="n">
         <v>509658.75</v>
       </c>
-      <c r="N231" t="inlineStr"/>
+      <c r="N231" t="inlineStr">
+        <is>
+          <t>货款</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="B232" t="inlineStr"/>
+      <c r="B232" s="2" t="n">
+        <v>43914</v>
+      </c>
       <c r="C232" t="inlineStr">
         <is>
           <t>2020-03-24 16:54:10</t>
@@ -10335,13 +11393,19 @@
       <c r="M232" t="n">
         <v>571658.75</v>
       </c>
-      <c r="N232" t="inlineStr"/>
+      <c r="N232" t="inlineStr">
+        <is>
+          <t>采购款</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
         <v>231</v>
       </c>
-      <c r="B233" t="inlineStr"/>
+      <c r="B233" s="2" t="n">
+        <v>43915</v>
+      </c>
       <c r="C233" t="inlineStr">
         <is>
           <t>2020-03-25 17:13:41</t>
@@ -10379,13 +11443,19 @@
       <c r="M233" t="n">
         <v>71658.75</v>
       </c>
-      <c r="N233" t="inlineStr"/>
+      <c r="N233" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="B234" t="inlineStr"/>
+      <c r="B234" s="2" t="n">
+        <v>43915</v>
+      </c>
       <c r="C234" t="inlineStr">
         <is>
           <t>2020-03-25 20:40:54</t>
@@ -10423,13 +11493,19 @@
       <c r="M234" t="n">
         <v>12858.75</v>
       </c>
-      <c r="N234" t="inlineStr"/>
+      <c r="N234" t="inlineStr">
+        <is>
+          <t>材料费</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="B235" t="inlineStr"/>
+      <c r="B235" s="2" t="n">
+        <v>43916</v>
+      </c>
       <c r="C235" t="inlineStr">
         <is>
           <t>2020-03-26 16:59:02</t>
@@ -10467,13 +11543,19 @@
       <c r="M235" t="n">
         <v>12213.75</v>
       </c>
-      <c r="N235" t="inlineStr"/>
+      <c r="N235" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
         <v>234</v>
       </c>
-      <c r="B236" t="inlineStr"/>
+      <c r="B236" s="2" t="n">
+        <v>43917</v>
+      </c>
       <c r="C236" t="inlineStr">
         <is>
           <t>2020-03-27 15:59:43</t>
@@ -10511,13 +11593,19 @@
       <c r="M236" t="n">
         <v>1172213.75</v>
       </c>
-      <c r="N236" t="inlineStr"/>
+      <c r="N236" t="inlineStr">
+        <is>
+          <t>一般往来款</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
         <v>235</v>
       </c>
-      <c r="B237" t="inlineStr"/>
+      <c r="B237" s="2" t="n">
+        <v>43917</v>
+      </c>
       <c r="C237" t="inlineStr">
         <is>
           <t>2020-03-27 16:22:41</t>
@@ -10555,13 +11643,19 @@
       <c r="M237" t="n">
         <v>1346105.64</v>
       </c>
-      <c r="N237" t="inlineStr"/>
+      <c r="N237" t="inlineStr">
+        <is>
+          <t>往来款</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="B238" t="inlineStr"/>
+      <c r="B238" s="2" t="n">
+        <v>43917</v>
+      </c>
       <c r="C238" t="inlineStr">
         <is>
           <t>2020-03-27 16:47:15</t>
@@ -10601,7 +11695,9 @@
       <c r="A239" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="B239" t="inlineStr"/>
+      <c r="B239" s="2" t="n">
+        <v>43917</v>
+      </c>
       <c r="C239" t="inlineStr">
         <is>
           <t>2020-03-27 17:02:29</t>
@@ -10639,13 +11735,19 @@
       <c r="M239" t="n">
         <v>1845841.66</v>
       </c>
-      <c r="N239" t="inlineStr"/>
+      <c r="N239" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="B240" t="inlineStr"/>
+      <c r="B240" s="2" t="n">
+        <v>43917</v>
+      </c>
       <c r="C240" t="inlineStr">
         <is>
           <t>2020-03-27 17:06:10</t>
@@ -10685,7 +11787,9 @@
       <c r="A241" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="B241" t="inlineStr"/>
+      <c r="B241" s="2" t="n">
+        <v>43918</v>
+      </c>
       <c r="C241" t="inlineStr">
         <is>
           <t>2020-03-28 09:29:45</t>
@@ -10723,13 +11827,19 @@
       <c r="M241" t="n">
         <v>431.66</v>
       </c>
-      <c r="N241" t="inlineStr"/>
+      <c r="N241" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="B242" t="inlineStr"/>
+      <c r="B242" s="2" t="n">
+        <v>43920</v>
+      </c>
       <c r="C242" t="inlineStr">
         <is>
           <t>2020-03-30 09:20:10</t>
@@ -10769,7 +11879,9 @@
       <c r="A243" s="1" t="n">
         <v>241</v>
       </c>
-      <c r="B243" t="inlineStr"/>
+      <c r="B243" s="2" t="n">
+        <v>43920</v>
+      </c>
       <c r="C243" t="inlineStr">
         <is>
           <t>2020-03-30 18:06:01</t>
@@ -10807,13 +11919,19 @@
       <c r="M243" t="n">
         <v>99904.60000000001</v>
       </c>
-      <c r="N243" t="inlineStr"/>
+      <c r="N243" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
         <v>242</v>
       </c>
-      <c r="B244" t="inlineStr"/>
+      <c r="B244" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C244" t="inlineStr">
         <is>
           <t>2020-03-31 08:59:20</t>
@@ -10851,13 +11969,19 @@
       <c r="M244" t="n">
         <v>99786.61</v>
       </c>
-      <c r="N244" t="inlineStr"/>
+      <c r="N244" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
         <v>243</v>
       </c>
-      <c r="B245" t="inlineStr"/>
+      <c r="B245" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C245" t="inlineStr">
         <is>
           <t>2020-03-31 14:17:16</t>
@@ -10895,13 +12019,19 @@
       <c r="M245" t="n">
         <v>226133.11</v>
       </c>
-      <c r="N245" t="inlineStr"/>
+      <c r="N245" t="inlineStr">
+        <is>
+          <t>采购款</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
         <v>244</v>
       </c>
-      <c r="B246" t="inlineStr"/>
+      <c r="B246" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C246" t="inlineStr">
         <is>
           <t>2020-03-31 15:37:01</t>
@@ -10939,13 +12069,19 @@
       <c r="M246" t="n">
         <v>426133.11</v>
       </c>
-      <c r="N246" t="inlineStr"/>
+      <c r="N246" t="inlineStr">
+        <is>
+          <t>借款</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
         <v>245</v>
       </c>
-      <c r="B247" t="inlineStr"/>
+      <c r="B247" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C247" t="inlineStr">
         <is>
           <t>2020-03-31 16:37:04</t>
@@ -10983,13 +12119,19 @@
       <c r="M247" t="n">
         <v>420736.11</v>
       </c>
-      <c r="N247" t="inlineStr"/>
+      <c r="N247" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
         <v>246</v>
       </c>
-      <c r="B248" t="inlineStr"/>
+      <c r="B248" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C248" t="inlineStr">
         <is>
           <t>2020-03-31 16:37:06</t>
@@ -11027,13 +12169,19 @@
       <c r="M248" t="n">
         <v>419599.11</v>
       </c>
-      <c r="N248" t="inlineStr"/>
+      <c r="N248" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
         <v>247</v>
       </c>
-      <c r="B249" t="inlineStr"/>
+      <c r="B249" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C249" t="inlineStr">
         <is>
           <t>2020-03-31 16:37:08</t>
@@ -11071,13 +12219,19 @@
       <c r="M249" t="n">
         <v>416099.11</v>
       </c>
-      <c r="N249" t="inlineStr"/>
+      <c r="N249" t="inlineStr">
+        <is>
+          <t>预支</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
         <v>248</v>
       </c>
-      <c r="B250" t="inlineStr"/>
+      <c r="B250" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C250" t="inlineStr">
         <is>
           <t>2020-03-31 16:37:09</t>
@@ -11115,13 +12269,19 @@
       <c r="M250" t="n">
         <v>411599.11</v>
       </c>
-      <c r="N250" t="inlineStr"/>
+      <c r="N250" t="inlineStr">
+        <is>
+          <t>材料费</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
         <v>249</v>
       </c>
-      <c r="B251" t="inlineStr"/>
+      <c r="B251" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C251" t="inlineStr">
         <is>
           <t>2020-03-31 16:37:11</t>
@@ -11159,13 +12319,19 @@
       <c r="M251" t="n">
         <v>410311.11</v>
       </c>
-      <c r="N251" t="inlineStr"/>
+      <c r="N251" t="inlineStr">
+        <is>
+          <t>报销</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="B252" t="inlineStr"/>
+      <c r="B252" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C252" t="inlineStr">
         <is>
           <t>2020-03-31 16:37:13</t>
@@ -11203,13 +12369,19 @@
       <c r="M252" t="n">
         <v>408636.71</v>
       </c>
-      <c r="N252" t="inlineStr"/>
+      <c r="N252" t="inlineStr">
+        <is>
+          <t>电费</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
         <v>251</v>
       </c>
-      <c r="B253" t="inlineStr"/>
+      <c r="B253" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C253" t="inlineStr">
         <is>
           <t>2020-03-31 18:01:54</t>
@@ -11249,7 +12421,9 @@
       <c r="A254" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="B254" t="inlineStr"/>
+      <c r="B254" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C254" t="inlineStr">
         <is>
           <t>2020-03-31 18:02:19</t>
@@ -11287,13 +12461,19 @@
       <c r="M254" t="n">
         <v>8643.379999999999</v>
       </c>
-      <c r="N254" t="inlineStr"/>
+      <c r="N254" t="inlineStr">
+        <is>
+          <t>转账开户转出账户</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
         <v>253</v>
       </c>
-      <c r="B255" t="inlineStr"/>
+      <c r="B255" s="2" t="n">
+        <v>43921</v>
+      </c>
       <c r="C255" t="inlineStr">
         <is>
           <t>2020-03-31 18:06:35</t>
@@ -11331,7 +12511,11 @@
       <c r="M255" t="n">
         <v>98643.38</v>
       </c>
-      <c r="N255" t="inlineStr"/>
+      <c r="N255" t="inlineStr">
+        <is>
+          <t>一般往来款</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>